<commit_message>
check with my rot coef
</commit_message>
<xml_diff>
--- a/docs/rot_coef_2048.xlsx
+++ b/docs/rot_coef_2048.xlsx
@@ -485,7 +485,7 @@
   <dimension ref="A1:N2049"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="N2" sqref="N2:N1537"/>
+      <selection activeCell="Q5" sqref="Q5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -558,8 +558,8 @@
       </c>
       <c r="M2" s="14"/>
       <c r="N2" s="15">
-        <f>IF((MOD(ROW(K2)-2,3)=0), K2, 9999)</f>
-        <v>0</v>
+        <f>IF((MOD(ROW(I2)-2,3)=0), I2, 9999)</f>
+        <v>1024</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
@@ -592,7 +592,7 @@
       </c>
       <c r="M3" s="14"/>
       <c r="N3" s="15">
-        <f t="shared" ref="N3:N66" si="6">IF((MOD(ROW(K3)-2,3)=0), K3, 9999)</f>
+        <f t="shared" ref="N3:N66" si="6">IF((MOD(ROW(I3)-2,3)=0), I3, 9999)</f>
         <v>9999</v>
       </c>
     </row>
@@ -661,7 +661,7 @@
       <c r="M5" s="14"/>
       <c r="N5" s="15">
         <f t="shared" si="6"/>
-        <v>9</v>
+        <v>1024</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
@@ -763,7 +763,7 @@
       <c r="M8" s="14"/>
       <c r="N8" s="15">
         <f t="shared" si="6"/>
-        <v>19</v>
+        <v>1024</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
@@ -875,7 +875,7 @@
       <c r="M11" s="14"/>
       <c r="N11" s="15">
         <f t="shared" si="6"/>
-        <v>28</v>
+        <v>1024</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
@@ -992,7 +992,7 @@
       <c r="M14" s="14"/>
       <c r="N14" s="15">
         <f t="shared" si="6"/>
-        <v>38</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
@@ -1109,7 +1109,7 @@
       <c r="M17" s="14"/>
       <c r="N17" s="15">
         <f t="shared" si="6"/>
-        <v>47</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
@@ -1221,7 +1221,7 @@
       <c r="M20" s="14"/>
       <c r="N20" s="15">
         <f t="shared" si="6"/>
-        <v>57</v>
+        <v>1022</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
@@ -1323,7 +1323,7 @@
       <c r="M23" s="14"/>
       <c r="N23" s="15">
         <f t="shared" si="6"/>
-        <v>66</v>
+        <v>1022</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
@@ -1425,7 +1425,7 @@
       <c r="M26" s="14"/>
       <c r="N26" s="15">
         <f t="shared" si="6"/>
-        <v>75</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
@@ -1527,7 +1527,7 @@
       <c r="M29" s="14"/>
       <c r="N29" s="15">
         <f t="shared" si="6"/>
-        <v>85</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
@@ -1629,7 +1629,7 @@
       <c r="M32" s="14"/>
       <c r="N32" s="15">
         <f t="shared" si="6"/>
-        <v>94</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
@@ -1731,7 +1731,7 @@
       <c r="M35" s="14"/>
       <c r="N35" s="15">
         <f t="shared" si="6"/>
-        <v>103</v>
+        <v>1019</v>
       </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
@@ -1833,7 +1833,7 @@
       <c r="M38" s="14"/>
       <c r="N38" s="15">
         <f t="shared" si="6"/>
-        <v>113</v>
+        <v>1018</v>
       </c>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.25">
@@ -1935,7 +1935,7 @@
       <c r="M41" s="14"/>
       <c r="N41" s="15">
         <f t="shared" si="6"/>
-        <v>122</v>
+        <v>1017</v>
       </c>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.25">
@@ -2037,7 +2037,7 @@
       <c r="M44" s="14"/>
       <c r="N44" s="15">
         <f t="shared" si="6"/>
-        <v>132</v>
+        <v>1016</v>
       </c>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.25">
@@ -2139,7 +2139,7 @@
       <c r="M47" s="14"/>
       <c r="N47" s="15">
         <f t="shared" si="6"/>
-        <v>141</v>
+        <v>1014</v>
       </c>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.25">
@@ -2241,7 +2241,7 @@
       <c r="M50" s="14"/>
       <c r="N50" s="15">
         <f t="shared" si="6"/>
-        <v>150</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.25">
@@ -2343,7 +2343,7 @@
       <c r="M53" s="14"/>
       <c r="N53" s="15">
         <f t="shared" si="6"/>
-        <v>160</v>
+        <v>1011</v>
       </c>
     </row>
     <row r="54" spans="1:14" x14ac:dyDescent="0.25">
@@ -2445,7 +2445,7 @@
       <c r="M56" s="14"/>
       <c r="N56" s="15">
         <f t="shared" si="6"/>
-        <v>169</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.25">
@@ -2547,7 +2547,7 @@
       <c r="M59" s="14"/>
       <c r="N59" s="15">
         <f t="shared" si="6"/>
-        <v>178</v>
+        <v>1008</v>
       </c>
     </row>
     <row r="60" spans="1:14" x14ac:dyDescent="0.25">
@@ -2649,7 +2649,7 @@
       <c r="M62" s="14"/>
       <c r="N62" s="15">
         <f t="shared" si="6"/>
-        <v>187</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="63" spans="1:14" x14ac:dyDescent="0.25">
@@ -2751,7 +2751,7 @@
       <c r="M65" s="14"/>
       <c r="N65" s="15">
         <f t="shared" si="6"/>
-        <v>197</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="66" spans="1:14" x14ac:dyDescent="0.25">
@@ -2818,7 +2818,7 @@
       </c>
       <c r="M67" s="14"/>
       <c r="N67" s="15">
-        <f t="shared" ref="N67:N130" si="13">IF((MOD(ROW(K67)-2,3)=0), K67, 9999)</f>
+        <f t="shared" ref="N67:N130" si="13">IF((MOD(ROW(I67)-2,3)=0), I67, 9999)</f>
         <v>9999</v>
       </c>
     </row>
@@ -2853,7 +2853,7 @@
       <c r="M68" s="14"/>
       <c r="N68" s="15">
         <f t="shared" si="13"/>
-        <v>206</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="69" spans="1:14" x14ac:dyDescent="0.25">
@@ -2955,7 +2955,7 @@
       <c r="M71" s="14"/>
       <c r="N71" s="15">
         <f t="shared" si="13"/>
-        <v>215</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="72" spans="1:14" x14ac:dyDescent="0.25">
@@ -3057,7 +3057,7 @@
       <c r="M74" s="14"/>
       <c r="N74" s="15">
         <f t="shared" si="13"/>
-        <v>224</v>
+        <v>999</v>
       </c>
     </row>
     <row r="75" spans="1:14" x14ac:dyDescent="0.25">
@@ -3159,7 +3159,7 @@
       <c r="M77" s="14"/>
       <c r="N77" s="15">
         <f t="shared" si="13"/>
-        <v>234</v>
+        <v>997</v>
       </c>
     </row>
     <row r="78" spans="1:14" x14ac:dyDescent="0.25">
@@ -3261,7 +3261,7 @@
       <c r="M80" s="14"/>
       <c r="N80" s="15">
         <f t="shared" si="13"/>
-        <v>243</v>
+        <v>995</v>
       </c>
     </row>
     <row r="81" spans="1:14" x14ac:dyDescent="0.25">
@@ -3363,7 +3363,7 @@
       <c r="M83" s="14"/>
       <c r="N83" s="15">
         <f t="shared" si="13"/>
-        <v>252</v>
+        <v>993</v>
       </c>
     </row>
     <row r="84" spans="1:14" x14ac:dyDescent="0.25">
@@ -3465,7 +3465,7 @@
       <c r="M86" s="14"/>
       <c r="N86" s="15">
         <f t="shared" si="13"/>
-        <v>261</v>
+        <v>990</v>
       </c>
     </row>
     <row r="87" spans="1:14" x14ac:dyDescent="0.25">
@@ -3567,7 +3567,7 @@
       <c r="M89" s="14"/>
       <c r="N89" s="15">
         <f t="shared" si="13"/>
-        <v>270</v>
+        <v>988</v>
       </c>
     </row>
     <row r="90" spans="1:14" x14ac:dyDescent="0.25">
@@ -3669,7 +3669,7 @@
       <c r="M92" s="14"/>
       <c r="N92" s="15">
         <f t="shared" si="13"/>
-        <v>279</v>
+        <v>985</v>
       </c>
     </row>
     <row r="93" spans="1:14" x14ac:dyDescent="0.25">
@@ -3771,7 +3771,7 @@
       <c r="M95" s="14"/>
       <c r="N95" s="15">
         <f t="shared" si="13"/>
-        <v>288</v>
+        <v>983</v>
       </c>
     </row>
     <row r="96" spans="1:14" x14ac:dyDescent="0.25">
@@ -3873,7 +3873,7 @@
       <c r="M98" s="14"/>
       <c r="N98" s="15">
         <f t="shared" si="13"/>
-        <v>297</v>
+        <v>980</v>
       </c>
     </row>
     <row r="99" spans="1:14" x14ac:dyDescent="0.25">
@@ -3975,7 +3975,7 @@
       <c r="M101" s="14"/>
       <c r="N101" s="15">
         <f t="shared" si="13"/>
-        <v>306</v>
+        <v>977</v>
       </c>
     </row>
     <row r="102" spans="1:14" x14ac:dyDescent="0.25">
@@ -4077,7 +4077,7 @@
       <c r="M104" s="14"/>
       <c r="N104" s="15">
         <f t="shared" si="13"/>
-        <v>315</v>
+        <v>974</v>
       </c>
     </row>
     <row r="105" spans="1:14" x14ac:dyDescent="0.25">
@@ -4179,7 +4179,7 @@
       <c r="M107" s="14"/>
       <c r="N107" s="15">
         <f t="shared" si="13"/>
-        <v>324</v>
+        <v>971</v>
       </c>
     </row>
     <row r="108" spans="1:14" x14ac:dyDescent="0.25">
@@ -4281,7 +4281,7 @@
       <c r="M110" s="14"/>
       <c r="N110" s="15">
         <f t="shared" si="13"/>
-        <v>333</v>
+        <v>968</v>
       </c>
     </row>
     <row r="111" spans="1:14" x14ac:dyDescent="0.25">
@@ -4383,7 +4383,7 @@
       <c r="M113" s="14"/>
       <c r="N113" s="15">
         <f t="shared" si="13"/>
-        <v>342</v>
+        <v>965</v>
       </c>
     </row>
     <row r="114" spans="1:14" x14ac:dyDescent="0.25">
@@ -4485,7 +4485,7 @@
       <c r="M116" s="14"/>
       <c r="N116" s="15">
         <f t="shared" si="13"/>
-        <v>351</v>
+        <v>962</v>
       </c>
     </row>
     <row r="117" spans="1:14" x14ac:dyDescent="0.25">
@@ -4587,7 +4587,7 @@
       <c r="M119" s="14"/>
       <c r="N119" s="15">
         <f t="shared" si="13"/>
-        <v>360</v>
+        <v>959</v>
       </c>
     </row>
     <row r="120" spans="1:14" x14ac:dyDescent="0.25">
@@ -4689,7 +4689,7 @@
       <c r="M122" s="14"/>
       <c r="N122" s="15">
         <f t="shared" si="13"/>
-        <v>369</v>
+        <v>955</v>
       </c>
     </row>
     <row r="123" spans="1:14" x14ac:dyDescent="0.25">
@@ -4791,7 +4791,7 @@
       <c r="M125" s="14"/>
       <c r="N125" s="15">
         <f t="shared" si="13"/>
-        <v>377</v>
+        <v>952</v>
       </c>
     </row>
     <row r="126" spans="1:14" x14ac:dyDescent="0.25">
@@ -4893,7 +4893,7 @@
       <c r="M128" s="14"/>
       <c r="N128" s="15">
         <f t="shared" si="13"/>
-        <v>386</v>
+        <v>948</v>
       </c>
     </row>
     <row r="129" spans="1:14" x14ac:dyDescent="0.25">
@@ -4994,8 +4994,8 @@
       </c>
       <c r="M131" s="14"/>
       <c r="N131" s="15">
-        <f t="shared" ref="N131:N194" si="20">IF((MOD(ROW(K131)-2,3)=0), K131, 9999)</f>
-        <v>395</v>
+        <f t="shared" ref="N131:N194" si="20">IF((MOD(ROW(I131)-2,3)=0), I131, 9999)</f>
+        <v>945</v>
       </c>
     </row>
     <row r="132" spans="1:14" x14ac:dyDescent="0.25">
@@ -5097,7 +5097,7 @@
       <c r="M134" s="14"/>
       <c r="N134" s="15">
         <f t="shared" si="20"/>
-        <v>403</v>
+        <v>941</v>
       </c>
     </row>
     <row r="135" spans="1:14" x14ac:dyDescent="0.25">
@@ -5199,7 +5199,7 @@
       <c r="M137" s="14"/>
       <c r="N137" s="15">
         <f t="shared" si="20"/>
-        <v>412</v>
+        <v>937</v>
       </c>
     </row>
     <row r="138" spans="1:14" x14ac:dyDescent="0.25">
@@ -5301,7 +5301,7 @@
       <c r="M140" s="14"/>
       <c r="N140" s="15">
         <f t="shared" si="20"/>
-        <v>421</v>
+        <v>934</v>
       </c>
     </row>
     <row r="141" spans="1:14" x14ac:dyDescent="0.25">
@@ -5403,7 +5403,7 @@
       <c r="M143" s="14"/>
       <c r="N143" s="15">
         <f t="shared" si="20"/>
-        <v>429</v>
+        <v>930</v>
       </c>
     </row>
     <row r="144" spans="1:14" x14ac:dyDescent="0.25">
@@ -5505,7 +5505,7 @@
       <c r="M146" s="14"/>
       <c r="N146" s="15">
         <f t="shared" si="20"/>
-        <v>438</v>
+        <v>926</v>
       </c>
     </row>
     <row r="147" spans="1:14" x14ac:dyDescent="0.25">
@@ -5607,7 +5607,7 @@
       <c r="M149" s="14"/>
       <c r="N149" s="15">
         <f t="shared" si="20"/>
-        <v>446</v>
+        <v>922</v>
       </c>
     </row>
     <row r="150" spans="1:14" x14ac:dyDescent="0.25">
@@ -5709,7 +5709,7 @@
       <c r="M152" s="14"/>
       <c r="N152" s="15">
         <f t="shared" si="20"/>
-        <v>455</v>
+        <v>917</v>
       </c>
     </row>
     <row r="153" spans="1:14" x14ac:dyDescent="0.25">
@@ -5811,7 +5811,7 @@
       <c r="M155" s="14"/>
       <c r="N155" s="15">
         <f t="shared" si="20"/>
-        <v>463</v>
+        <v>913</v>
       </c>
     </row>
     <row r="156" spans="1:14" x14ac:dyDescent="0.25">
@@ -5913,7 +5913,7 @@
       <c r="M158" s="14"/>
       <c r="N158" s="15">
         <f t="shared" si="20"/>
-        <v>472</v>
+        <v>909</v>
       </c>
     </row>
     <row r="159" spans="1:14" x14ac:dyDescent="0.25">
@@ -6015,7 +6015,7 @@
       <c r="M161" s="14"/>
       <c r="N161" s="15">
         <f t="shared" si="20"/>
-        <v>480</v>
+        <v>905</v>
       </c>
     </row>
     <row r="162" spans="1:14" x14ac:dyDescent="0.25">
@@ -6117,7 +6117,7 @@
       <c r="M164" s="14"/>
       <c r="N164" s="15">
         <f t="shared" si="20"/>
-        <v>488</v>
+        <v>900</v>
       </c>
     </row>
     <row r="165" spans="1:14" x14ac:dyDescent="0.25">
@@ -6219,7 +6219,7 @@
       <c r="M167" s="14"/>
       <c r="N167" s="15">
         <f t="shared" si="20"/>
-        <v>497</v>
+        <v>896</v>
       </c>
     </row>
     <row r="168" spans="1:14" x14ac:dyDescent="0.25">
@@ -6321,7 +6321,7 @@
       <c r="M170" s="14"/>
       <c r="N170" s="15">
         <f t="shared" si="20"/>
-        <v>505</v>
+        <v>891</v>
       </c>
     </row>
     <row r="171" spans="1:14" x14ac:dyDescent="0.25">
@@ -6423,7 +6423,7 @@
       <c r="M173" s="14"/>
       <c r="N173" s="15">
         <f t="shared" si="20"/>
-        <v>513</v>
+        <v>886</v>
       </c>
     </row>
     <row r="174" spans="1:14" x14ac:dyDescent="0.25">
@@ -6525,7 +6525,7 @@
       <c r="M176" s="14"/>
       <c r="N176" s="15">
         <f t="shared" si="20"/>
-        <v>521</v>
+        <v>882</v>
       </c>
     </row>
     <row r="177" spans="1:14" x14ac:dyDescent="0.25">
@@ -6627,7 +6627,7 @@
       <c r="M179" s="14"/>
       <c r="N179" s="15">
         <f t="shared" si="20"/>
-        <v>529</v>
+        <v>877</v>
       </c>
     </row>
     <row r="180" spans="1:14" x14ac:dyDescent="0.25">
@@ -6729,7 +6729,7 @@
       <c r="M182" s="14"/>
       <c r="N182" s="15">
         <f t="shared" si="20"/>
-        <v>537</v>
+        <v>872</v>
       </c>
     </row>
     <row r="183" spans="1:14" x14ac:dyDescent="0.25">
@@ -6831,7 +6831,7 @@
       <c r="M185" s="14"/>
       <c r="N185" s="15">
         <f t="shared" si="20"/>
-        <v>545</v>
+        <v>867</v>
       </c>
     </row>
     <row r="186" spans="1:14" x14ac:dyDescent="0.25">
@@ -6933,7 +6933,7 @@
       <c r="M188" s="14"/>
       <c r="N188" s="15">
         <f t="shared" si="20"/>
-        <v>553</v>
+        <v>862</v>
       </c>
     </row>
     <row r="189" spans="1:14" x14ac:dyDescent="0.25">
@@ -7035,7 +7035,7 @@
       <c r="M191" s="14"/>
       <c r="N191" s="15">
         <f t="shared" si="20"/>
-        <v>561</v>
+        <v>857</v>
       </c>
     </row>
     <row r="192" spans="1:14" x14ac:dyDescent="0.25">
@@ -7137,7 +7137,7 @@
       <c r="M194" s="14"/>
       <c r="N194" s="15">
         <f t="shared" si="20"/>
-        <v>569</v>
+        <v>851</v>
       </c>
     </row>
     <row r="195" spans="1:14" x14ac:dyDescent="0.25">
@@ -7170,7 +7170,7 @@
       </c>
       <c r="M195" s="14"/>
       <c r="N195" s="15">
-        <f t="shared" ref="N195:N258" si="27">IF((MOD(ROW(K195)-2,3)=0), K195, 9999)</f>
+        <f t="shared" ref="N195:N258" si="27">IF((MOD(ROW(I195)-2,3)=0), I195, 9999)</f>
         <v>9999</v>
       </c>
     </row>
@@ -7239,7 +7239,7 @@
       <c r="M197" s="14"/>
       <c r="N197" s="15">
         <f t="shared" si="27"/>
-        <v>577</v>
+        <v>846</v>
       </c>
     </row>
     <row r="198" spans="1:14" x14ac:dyDescent="0.25">
@@ -7341,7 +7341,7 @@
       <c r="M200" s="14"/>
       <c r="N200" s="15">
         <f t="shared" si="27"/>
-        <v>584</v>
+        <v>841</v>
       </c>
     </row>
     <row r="201" spans="1:14" x14ac:dyDescent="0.25">
@@ -7443,7 +7443,7 @@
       <c r="M203" s="14"/>
       <c r="N203" s="15">
         <f t="shared" si="27"/>
-        <v>592</v>
+        <v>835</v>
       </c>
     </row>
     <row r="204" spans="1:14" x14ac:dyDescent="0.25">
@@ -7545,7 +7545,7 @@
       <c r="M206" s="14"/>
       <c r="N206" s="15">
         <f t="shared" si="27"/>
-        <v>600</v>
+        <v>830</v>
       </c>
     </row>
     <row r="207" spans="1:14" x14ac:dyDescent="0.25">
@@ -7647,7 +7647,7 @@
       <c r="M209" s="14"/>
       <c r="N209" s="15">
         <f t="shared" si="27"/>
-        <v>607</v>
+        <v>824</v>
       </c>
     </row>
     <row r="210" spans="1:14" x14ac:dyDescent="0.25">
@@ -7749,7 +7749,7 @@
       <c r="M212" s="14"/>
       <c r="N212" s="15">
         <f t="shared" si="27"/>
-        <v>615</v>
+        <v>819</v>
       </c>
     </row>
     <row r="213" spans="1:14" x14ac:dyDescent="0.25">
@@ -7851,7 +7851,7 @@
       <c r="M215" s="14"/>
       <c r="N215" s="15">
         <f t="shared" si="27"/>
-        <v>623</v>
+        <v>813</v>
       </c>
     </row>
     <row r="216" spans="1:14" x14ac:dyDescent="0.25">
@@ -7953,7 +7953,7 @@
       <c r="M218" s="14"/>
       <c r="N218" s="15">
         <f t="shared" si="27"/>
-        <v>630</v>
+        <v>807</v>
       </c>
     </row>
     <row r="219" spans="1:14" x14ac:dyDescent="0.25">
@@ -8055,7 +8055,7 @@
       <c r="M221" s="14"/>
       <c r="N221" s="15">
         <f t="shared" si="27"/>
-        <v>637</v>
+        <v>801</v>
       </c>
     </row>
     <row r="222" spans="1:14" x14ac:dyDescent="0.25">
@@ -8157,7 +8157,7 @@
       <c r="M224" s="14"/>
       <c r="N224" s="15">
         <f t="shared" si="27"/>
-        <v>645</v>
+        <v>796</v>
       </c>
     </row>
     <row r="225" spans="1:14" x14ac:dyDescent="0.25">
@@ -8259,7 +8259,7 @@
       <c r="M227" s="14"/>
       <c r="N227" s="15">
         <f t="shared" si="27"/>
-        <v>652</v>
+        <v>790</v>
       </c>
     </row>
     <row r="228" spans="1:14" x14ac:dyDescent="0.25">
@@ -8361,7 +8361,7 @@
       <c r="M230" s="14"/>
       <c r="N230" s="15">
         <f t="shared" si="27"/>
-        <v>659</v>
+        <v>784</v>
       </c>
     </row>
     <row r="231" spans="1:14" x14ac:dyDescent="0.25">
@@ -8463,7 +8463,7 @@
       <c r="M233" s="14"/>
       <c r="N233" s="15">
         <f t="shared" si="27"/>
-        <v>666</v>
+        <v>777</v>
       </c>
     </row>
     <row r="234" spans="1:14" x14ac:dyDescent="0.25">
@@ -8565,7 +8565,7 @@
       <c r="M236" s="14"/>
       <c r="N236" s="15">
         <f t="shared" si="27"/>
-        <v>674</v>
+        <v>771</v>
       </c>
     </row>
     <row r="237" spans="1:14" x14ac:dyDescent="0.25">
@@ -8667,7 +8667,7 @@
       <c r="M239" s="14"/>
       <c r="N239" s="15">
         <f t="shared" si="27"/>
-        <v>681</v>
+        <v>765</v>
       </c>
     </row>
     <row r="240" spans="1:14" x14ac:dyDescent="0.25">
@@ -8769,7 +8769,7 @@
       <c r="M242" s="14"/>
       <c r="N242" s="15">
         <f t="shared" si="27"/>
-        <v>688</v>
+        <v>759</v>
       </c>
     </row>
     <row r="243" spans="1:14" x14ac:dyDescent="0.25">
@@ -8871,7 +8871,7 @@
       <c r="M245" s="14"/>
       <c r="N245" s="15">
         <f t="shared" si="27"/>
-        <v>695</v>
+        <v>752</v>
       </c>
     </row>
     <row r="246" spans="1:14" x14ac:dyDescent="0.25">
@@ -8973,7 +8973,7 @@
       <c r="M248" s="14"/>
       <c r="N248" s="15">
         <f t="shared" si="27"/>
-        <v>702</v>
+        <v>746</v>
       </c>
     </row>
     <row r="249" spans="1:14" x14ac:dyDescent="0.25">
@@ -9075,7 +9075,7 @@
       <c r="M251" s="14"/>
       <c r="N251" s="15">
         <f t="shared" si="27"/>
-        <v>708</v>
+        <v>739</v>
       </c>
     </row>
     <row r="252" spans="1:14" x14ac:dyDescent="0.25">
@@ -9177,7 +9177,7 @@
       <c r="M254" s="14"/>
       <c r="N254" s="15">
         <f t="shared" si="27"/>
-        <v>715</v>
+        <v>733</v>
       </c>
     </row>
     <row r="255" spans="1:14" x14ac:dyDescent="0.25">
@@ -9279,7 +9279,7 @@
       <c r="M257" s="14"/>
       <c r="N257" s="15">
         <f t="shared" si="27"/>
-        <v>722</v>
+        <v>726</v>
       </c>
     </row>
     <row r="258" spans="1:14" x14ac:dyDescent="0.25">
@@ -9354,7 +9354,7 @@
         <v>2D6</v>
       </c>
       <c r="N259" s="15">
-        <f t="shared" ref="N259:N322" si="34">IF((MOD(ROW(K259)-2,3)=0), K259, 9999)</f>
+        <f t="shared" ref="N259:N322" si="34">IF((MOD(ROW(I259)-2,3)=0), I259, 9999)</f>
         <v>9999</v>
       </c>
     </row>
@@ -9393,7 +9393,7 @@
       </c>
       <c r="N260" s="15">
         <f t="shared" si="34"/>
-        <v>729</v>
+        <v>720</v>
       </c>
     </row>
     <row r="261" spans="1:14" x14ac:dyDescent="0.25">
@@ -9507,7 +9507,7 @@
       </c>
       <c r="N263" s="15">
         <f t="shared" si="34"/>
-        <v>735</v>
+        <v>713</v>
       </c>
     </row>
     <row r="264" spans="1:14" x14ac:dyDescent="0.25">
@@ -9621,7 +9621,7 @@
       </c>
       <c r="N266" s="15">
         <f t="shared" si="34"/>
-        <v>742</v>
+        <v>706</v>
       </c>
     </row>
     <row r="267" spans="1:14" x14ac:dyDescent="0.25">
@@ -9735,7 +9735,7 @@
       </c>
       <c r="N269" s="15">
         <f t="shared" si="34"/>
-        <v>748</v>
+        <v>699</v>
       </c>
     </row>
     <row r="270" spans="1:14" x14ac:dyDescent="0.25">
@@ -9849,7 +9849,7 @@
       </c>
       <c r="N272" s="15">
         <f t="shared" si="34"/>
-        <v>755</v>
+        <v>692</v>
       </c>
     </row>
     <row r="273" spans="1:14" x14ac:dyDescent="0.25">
@@ -9963,7 +9963,7 @@
       </c>
       <c r="N275" s="15">
         <f t="shared" si="34"/>
-        <v>761</v>
+        <v>685</v>
       </c>
     </row>
     <row r="276" spans="1:14" x14ac:dyDescent="0.25">
@@ -10077,7 +10077,7 @@
       </c>
       <c r="N278" s="15">
         <f t="shared" si="34"/>
-        <v>767</v>
+        <v>678</v>
       </c>
     </row>
     <row r="279" spans="1:14" x14ac:dyDescent="0.25">
@@ -10191,7 +10191,7 @@
       </c>
       <c r="N281" s="15">
         <f t="shared" si="34"/>
-        <v>773</v>
+        <v>671</v>
       </c>
     </row>
     <row r="282" spans="1:14" x14ac:dyDescent="0.25">
@@ -10305,7 +10305,7 @@
       </c>
       <c r="N284" s="15">
         <f t="shared" si="34"/>
-        <v>779</v>
+        <v>664</v>
       </c>
     </row>
     <row r="285" spans="1:14" x14ac:dyDescent="0.25">
@@ -10419,7 +10419,7 @@
       </c>
       <c r="N287" s="15">
         <f t="shared" si="34"/>
-        <v>786</v>
+        <v>657</v>
       </c>
     </row>
     <row r="288" spans="1:14" x14ac:dyDescent="0.25">
@@ -10533,7 +10533,7 @@
       </c>
       <c r="N290" s="15">
         <f t="shared" si="34"/>
-        <v>792</v>
+        <v>650</v>
       </c>
     </row>
     <row r="291" spans="1:14" x14ac:dyDescent="0.25">
@@ -10647,7 +10647,7 @@
       </c>
       <c r="N293" s="15">
         <f t="shared" si="34"/>
-        <v>798</v>
+        <v>642</v>
       </c>
     </row>
     <row r="294" spans="1:14" x14ac:dyDescent="0.25">
@@ -10761,7 +10761,7 @@
       </c>
       <c r="N296" s="15">
         <f t="shared" si="34"/>
-        <v>803</v>
+        <v>635</v>
       </c>
     </row>
     <row r="297" spans="1:14" x14ac:dyDescent="0.25">
@@ -10875,7 +10875,7 @@
       </c>
       <c r="N299" s="15">
         <f t="shared" si="34"/>
-        <v>809</v>
+        <v>628</v>
       </c>
     </row>
     <row r="300" spans="1:14" x14ac:dyDescent="0.25">
@@ -10989,7 +10989,7 @@
       </c>
       <c r="N302" s="15">
         <f t="shared" si="34"/>
-        <v>815</v>
+        <v>620</v>
       </c>
     </row>
     <row r="303" spans="1:14" x14ac:dyDescent="0.25">
@@ -11103,7 +11103,7 @@
       </c>
       <c r="N305" s="15">
         <f t="shared" si="34"/>
-        <v>821</v>
+        <v>613</v>
       </c>
     </row>
     <row r="306" spans="1:14" x14ac:dyDescent="0.25">
@@ -11217,7 +11217,7 @@
       </c>
       <c r="N308" s="15">
         <f t="shared" si="34"/>
-        <v>826</v>
+        <v>605</v>
       </c>
     </row>
     <row r="309" spans="1:14" x14ac:dyDescent="0.25">
@@ -11331,7 +11331,7 @@
       </c>
       <c r="N311" s="15">
         <f t="shared" si="34"/>
-        <v>832</v>
+        <v>597</v>
       </c>
     </row>
     <row r="312" spans="1:14" x14ac:dyDescent="0.25">
@@ -11445,7 +11445,7 @@
       </c>
       <c r="N314" s="15">
         <f t="shared" si="34"/>
-        <v>837</v>
+        <v>590</v>
       </c>
     </row>
     <row r="315" spans="1:14" x14ac:dyDescent="0.25">
@@ -11559,7 +11559,7 @@
       </c>
       <c r="N317" s="15">
         <f t="shared" si="34"/>
-        <v>843</v>
+        <v>582</v>
       </c>
     </row>
     <row r="318" spans="1:14" x14ac:dyDescent="0.25">
@@ -11673,7 +11673,7 @@
       </c>
       <c r="N320" s="15">
         <f t="shared" si="34"/>
-        <v>848</v>
+        <v>574</v>
       </c>
     </row>
     <row r="321" spans="1:14" x14ac:dyDescent="0.25">
@@ -11786,8 +11786,8 @@
         <v>355</v>
       </c>
       <c r="N323" s="15">
-        <f t="shared" ref="N323:N386" si="41">IF((MOD(ROW(K323)-2,3)=0), K323, 9999)</f>
-        <v>853</v>
+        <f t="shared" ref="N323:N386" si="41">IF((MOD(ROW(I323)-2,3)=0), I323, 9999)</f>
+        <v>566</v>
       </c>
     </row>
     <row r="324" spans="1:14" x14ac:dyDescent="0.25">
@@ -11901,7 +11901,7 @@
       </c>
       <c r="N326" s="15">
         <f t="shared" si="41"/>
-        <v>858</v>
+        <v>558</v>
       </c>
     </row>
     <row r="327" spans="1:14" x14ac:dyDescent="0.25">
@@ -12015,7 +12015,7 @@
       </c>
       <c r="N329" s="15">
         <f t="shared" si="41"/>
-        <v>863</v>
+        <v>550</v>
       </c>
     </row>
     <row r="330" spans="1:14" x14ac:dyDescent="0.25">
@@ -12129,7 +12129,7 @@
       </c>
       <c r="N332" s="15">
         <f t="shared" si="41"/>
-        <v>868</v>
+        <v>543</v>
       </c>
     </row>
     <row r="333" spans="1:14" x14ac:dyDescent="0.25">
@@ -12243,7 +12243,7 @@
       </c>
       <c r="N335" s="15">
         <f t="shared" si="41"/>
-        <v>873</v>
+        <v>535</v>
       </c>
     </row>
     <row r="336" spans="1:14" x14ac:dyDescent="0.25">
@@ -12357,7 +12357,7 @@
       </c>
       <c r="N338" s="15">
         <f t="shared" si="41"/>
-        <v>878</v>
+        <v>526</v>
       </c>
     </row>
     <row r="339" spans="1:14" x14ac:dyDescent="0.25">
@@ -12471,7 +12471,7 @@
       </c>
       <c r="N341" s="15">
         <f t="shared" si="41"/>
-        <v>883</v>
+        <v>518</v>
       </c>
     </row>
     <row r="342" spans="1:14" x14ac:dyDescent="0.25">
@@ -12585,7 +12585,7 @@
       </c>
       <c r="N344" s="15">
         <f t="shared" si="41"/>
-        <v>888</v>
+        <v>510</v>
       </c>
     </row>
     <row r="345" spans="1:14" x14ac:dyDescent="0.25">
@@ -12699,7 +12699,7 @@
       </c>
       <c r="N347" s="15">
         <f t="shared" si="41"/>
-        <v>893</v>
+        <v>502</v>
       </c>
     </row>
     <row r="348" spans="1:14" x14ac:dyDescent="0.25">
@@ -12813,7 +12813,7 @@
       </c>
       <c r="N350" s="15">
         <f t="shared" si="41"/>
-        <v>897</v>
+        <v>494</v>
       </c>
     </row>
     <row r="351" spans="1:14" x14ac:dyDescent="0.25">
@@ -12927,7 +12927,7 @@
       </c>
       <c r="N353" s="15">
         <f t="shared" si="41"/>
-        <v>902</v>
+        <v>485</v>
       </c>
     </row>
     <row r="354" spans="1:14" x14ac:dyDescent="0.25">
@@ -13041,7 +13041,7 @@
       </c>
       <c r="N356" s="15">
         <f t="shared" si="41"/>
-        <v>906</v>
+        <v>477</v>
       </c>
     </row>
     <row r="357" spans="1:14" x14ac:dyDescent="0.25">
@@ -13155,7 +13155,7 @@
       </c>
       <c r="N359" s="15">
         <f t="shared" si="41"/>
-        <v>910</v>
+        <v>469</v>
       </c>
     </row>
     <row r="360" spans="1:14" x14ac:dyDescent="0.25">
@@ -13269,7 +13269,7 @@
       </c>
       <c r="N362" s="15">
         <f t="shared" si="41"/>
-        <v>915</v>
+        <v>460</v>
       </c>
     </row>
     <row r="363" spans="1:14" x14ac:dyDescent="0.25">
@@ -13383,7 +13383,7 @@
       </c>
       <c r="N365" s="15">
         <f t="shared" si="41"/>
-        <v>919</v>
+        <v>452</v>
       </c>
     </row>
     <row r="366" spans="1:14" x14ac:dyDescent="0.25">
@@ -13497,7 +13497,7 @@
       </c>
       <c r="N368" s="15">
         <f t="shared" si="41"/>
-        <v>923</v>
+        <v>443</v>
       </c>
     </row>
     <row r="369" spans="1:14" x14ac:dyDescent="0.25">
@@ -13611,7 +13611,7 @@
       </c>
       <c r="N371" s="15">
         <f t="shared" si="41"/>
-        <v>927</v>
+        <v>435</v>
       </c>
     </row>
     <row r="372" spans="1:14" x14ac:dyDescent="0.25">
@@ -13725,7 +13725,7 @@
       </c>
       <c r="N374" s="15">
         <f t="shared" si="41"/>
-        <v>931</v>
+        <v>426</v>
       </c>
     </row>
     <row r="375" spans="1:14" x14ac:dyDescent="0.25">
@@ -13839,7 +13839,7 @@
       </c>
       <c r="N377" s="15">
         <f t="shared" si="41"/>
-        <v>935</v>
+        <v>418</v>
       </c>
     </row>
     <row r="378" spans="1:14" x14ac:dyDescent="0.25">
@@ -13953,7 +13953,7 @@
       </c>
       <c r="N380" s="15">
         <f t="shared" si="41"/>
-        <v>939</v>
+        <v>409</v>
       </c>
     </row>
     <row r="381" spans="1:14" x14ac:dyDescent="0.25">
@@ -14067,7 +14067,7 @@
       </c>
       <c r="N383" s="15">
         <f t="shared" si="41"/>
-        <v>942</v>
+        <v>401</v>
       </c>
     </row>
     <row r="384" spans="1:14" x14ac:dyDescent="0.25">
@@ -14181,7 +14181,7 @@
       </c>
       <c r="N386" s="15">
         <f t="shared" si="41"/>
-        <v>946</v>
+        <v>392</v>
       </c>
     </row>
     <row r="387" spans="1:14" x14ac:dyDescent="0.25">
@@ -14218,7 +14218,7 @@
         <v>3B3</v>
       </c>
       <c r="N387" s="15">
-        <f t="shared" ref="N387:N450" si="48">IF((MOD(ROW(K387)-2,3)=0), K387, 9999)</f>
+        <f t="shared" ref="N387:N450" si="48">IF((MOD(ROW(I387)-2,3)=0), I387, 9999)</f>
         <v>9999</v>
       </c>
     </row>
@@ -14295,7 +14295,7 @@
       </c>
       <c r="N389" s="15">
         <f t="shared" si="48"/>
-        <v>950</v>
+        <v>383</v>
       </c>
     </row>
     <row r="390" spans="1:14" x14ac:dyDescent="0.25">
@@ -14409,7 +14409,7 @@
       </c>
       <c r="N392" s="15">
         <f t="shared" si="48"/>
-        <v>953</v>
+        <v>374</v>
       </c>
     </row>
     <row r="393" spans="1:14" x14ac:dyDescent="0.25">
@@ -14523,7 +14523,7 @@
       </c>
       <c r="N395" s="15">
         <f t="shared" si="48"/>
-        <v>957</v>
+        <v>366</v>
       </c>
     </row>
     <row r="396" spans="1:14" x14ac:dyDescent="0.25">
@@ -14637,7 +14637,7 @@
       </c>
       <c r="N398" s="15">
         <f t="shared" si="48"/>
-        <v>960</v>
+        <v>357</v>
       </c>
     </row>
     <row r="399" spans="1:14" x14ac:dyDescent="0.25">
@@ -14751,7 +14751,7 @@
       </c>
       <c r="N401" s="15">
         <f t="shared" si="48"/>
-        <v>963</v>
+        <v>348</v>
       </c>
     </row>
     <row r="402" spans="1:14" x14ac:dyDescent="0.25">
@@ -14865,7 +14865,7 @@
       </c>
       <c r="N404" s="15">
         <f t="shared" si="48"/>
-        <v>966</v>
+        <v>339</v>
       </c>
     </row>
     <row r="405" spans="1:14" x14ac:dyDescent="0.25">
@@ -14979,7 +14979,7 @@
       </c>
       <c r="N407" s="15">
         <f t="shared" si="48"/>
-        <v>969</v>
+        <v>330</v>
       </c>
     </row>
     <row r="408" spans="1:14" x14ac:dyDescent="0.25">
@@ -15093,7 +15093,7 @@
       </c>
       <c r="N410" s="15">
         <f t="shared" si="48"/>
-        <v>972</v>
+        <v>321</v>
       </c>
     </row>
     <row r="411" spans="1:14" x14ac:dyDescent="0.25">
@@ -15207,7 +15207,7 @@
       </c>
       <c r="N413" s="15">
         <f t="shared" si="48"/>
-        <v>975</v>
+        <v>312</v>
       </c>
     </row>
     <row r="414" spans="1:14" x14ac:dyDescent="0.25">
@@ -15321,7 +15321,7 @@
       </c>
       <c r="N416" s="15">
         <f t="shared" si="48"/>
-        <v>978</v>
+        <v>303</v>
       </c>
     </row>
     <row r="417" spans="1:14" x14ac:dyDescent="0.25">
@@ -15435,7 +15435,7 @@
       </c>
       <c r="N419" s="15">
         <f t="shared" si="48"/>
-        <v>981</v>
+        <v>294</v>
       </c>
     </row>
     <row r="420" spans="1:14" x14ac:dyDescent="0.25">
@@ -15549,7 +15549,7 @@
       </c>
       <c r="N422" s="15">
         <f t="shared" si="48"/>
-        <v>983</v>
+        <v>285</v>
       </c>
     </row>
     <row r="423" spans="1:14" x14ac:dyDescent="0.25">
@@ -15663,7 +15663,7 @@
       </c>
       <c r="N425" s="15">
         <f t="shared" si="48"/>
-        <v>986</v>
+        <v>276</v>
       </c>
     </row>
     <row r="426" spans="1:14" x14ac:dyDescent="0.25">
@@ -15777,7 +15777,7 @@
       </c>
       <c r="N428" s="15">
         <f t="shared" si="48"/>
-        <v>989</v>
+        <v>267</v>
       </c>
     </row>
     <row r="429" spans="1:14" x14ac:dyDescent="0.25">
@@ -15891,7 +15891,7 @@
       </c>
       <c r="N431" s="15">
         <f t="shared" si="48"/>
-        <v>991</v>
+        <v>258</v>
       </c>
     </row>
     <row r="432" spans="1:14" x14ac:dyDescent="0.25">
@@ -16005,7 +16005,7 @@
       </c>
       <c r="N434" s="15">
         <f t="shared" si="48"/>
-        <v>993</v>
+        <v>249</v>
       </c>
     </row>
     <row r="435" spans="1:14" x14ac:dyDescent="0.25">
@@ -16119,7 +16119,7 @@
       </c>
       <c r="N437" s="15">
         <f t="shared" si="48"/>
-        <v>996</v>
+        <v>240</v>
       </c>
     </row>
     <row r="438" spans="1:14" x14ac:dyDescent="0.25">
@@ -16233,7 +16233,7 @@
       </c>
       <c r="N440" s="15">
         <f t="shared" si="48"/>
-        <v>998</v>
+        <v>230</v>
       </c>
     </row>
     <row r="441" spans="1:14" x14ac:dyDescent="0.25">
@@ -16347,7 +16347,7 @@
       </c>
       <c r="N443" s="15">
         <f t="shared" si="48"/>
-        <v>1000</v>
+        <v>221</v>
       </c>
     </row>
     <row r="444" spans="1:14" x14ac:dyDescent="0.25">
@@ -16461,7 +16461,7 @@
       </c>
       <c r="N446" s="15">
         <f t="shared" si="48"/>
-        <v>1002</v>
+        <v>212</v>
       </c>
     </row>
     <row r="447" spans="1:14" x14ac:dyDescent="0.25">
@@ -16575,7 +16575,7 @@
       </c>
       <c r="N449" s="15">
         <f t="shared" si="48"/>
-        <v>1004</v>
+        <v>203</v>
       </c>
     </row>
     <row r="450" spans="1:14" x14ac:dyDescent="0.25">
@@ -16650,7 +16650,7 @@
         <v>3ED</v>
       </c>
       <c r="N451" s="15">
-        <f t="shared" ref="N451:N514" si="55">IF((MOD(ROW(K451)-2,3)=0), K451, 9999)</f>
+        <f t="shared" ref="N451:N514" si="55">IF((MOD(ROW(I451)-2,3)=0), I451, 9999)</f>
         <v>9999</v>
       </c>
     </row>
@@ -16689,7 +16689,7 @@
       </c>
       <c r="N452" s="15">
         <f t="shared" si="55"/>
-        <v>1006</v>
+        <v>194</v>
       </c>
     </row>
     <row r="453" spans="1:14" x14ac:dyDescent="0.25">
@@ -16803,7 +16803,7 @@
       </c>
       <c r="N455" s="15">
         <f t="shared" si="55"/>
-        <v>1007</v>
+        <v>184</v>
       </c>
     </row>
     <row r="456" spans="1:14" x14ac:dyDescent="0.25">
@@ -16917,7 +16917,7 @@
       </c>
       <c r="N458" s="15">
         <f t="shared" si="55"/>
-        <v>1009</v>
+        <v>175</v>
       </c>
     </row>
     <row r="459" spans="1:14" x14ac:dyDescent="0.25">
@@ -17031,7 +17031,7 @@
       </c>
       <c r="N461" s="15">
         <f t="shared" si="55"/>
-        <v>1010</v>
+        <v>166</v>
       </c>
     </row>
     <row r="462" spans="1:14" x14ac:dyDescent="0.25">
@@ -17145,7 +17145,7 @@
       </c>
       <c r="N464" s="15">
         <f t="shared" si="55"/>
-        <v>1012</v>
+        <v>156</v>
       </c>
     </row>
     <row r="465" spans="1:14" x14ac:dyDescent="0.25">
@@ -17259,7 +17259,7 @@
       </c>
       <c r="N467" s="15">
         <f t="shared" si="55"/>
-        <v>1013</v>
+        <v>147</v>
       </c>
     </row>
     <row r="468" spans="1:14" x14ac:dyDescent="0.25">
@@ -17373,7 +17373,7 @@
       </c>
       <c r="N470" s="15">
         <f t="shared" si="55"/>
-        <v>1015</v>
+        <v>138</v>
       </c>
     </row>
     <row r="471" spans="1:14" x14ac:dyDescent="0.25">
@@ -17487,7 +17487,7 @@
       </c>
       <c r="N473" s="15">
         <f t="shared" si="55"/>
-        <v>1016</v>
+        <v>128</v>
       </c>
     </row>
     <row r="474" spans="1:14" x14ac:dyDescent="0.25">
@@ -17601,7 +17601,7 @@
       </c>
       <c r="N476" s="15">
         <f t="shared" si="55"/>
-        <v>1017</v>
+        <v>119</v>
       </c>
     </row>
     <row r="477" spans="1:14" x14ac:dyDescent="0.25">
@@ -17715,7 +17715,7 @@
       </c>
       <c r="N479" s="15">
         <f t="shared" si="55"/>
-        <v>1018</v>
+        <v>110</v>
       </c>
     </row>
     <row r="480" spans="1:14" x14ac:dyDescent="0.25">
@@ -17829,7 +17829,7 @@
       </c>
       <c r="N482" s="15">
         <f t="shared" si="55"/>
-        <v>1019</v>
+        <v>100</v>
       </c>
     </row>
     <row r="483" spans="1:14" x14ac:dyDescent="0.25">
@@ -17943,7 +17943,7 @@
       </c>
       <c r="N485" s="15">
         <f t="shared" si="55"/>
-        <v>1020</v>
+        <v>91</v>
       </c>
     </row>
     <row r="486" spans="1:14" x14ac:dyDescent="0.25">
@@ -18057,7 +18057,7 @@
       </c>
       <c r="N488" s="15">
         <f t="shared" si="55"/>
-        <v>1021</v>
+        <v>82</v>
       </c>
     </row>
     <row r="489" spans="1:14" x14ac:dyDescent="0.25">
@@ -18171,7 +18171,7 @@
       </c>
       <c r="N491" s="15">
         <f t="shared" si="55"/>
-        <v>1021</v>
+        <v>72</v>
       </c>
     </row>
     <row r="492" spans="1:14" x14ac:dyDescent="0.25">
@@ -18285,7 +18285,7 @@
       </c>
       <c r="N494" s="15">
         <f t="shared" si="55"/>
-        <v>1022</v>
+        <v>63</v>
       </c>
     </row>
     <row r="495" spans="1:14" x14ac:dyDescent="0.25">
@@ -18399,7 +18399,7 @@
       </c>
       <c r="N497" s="15">
         <f t="shared" si="55"/>
-        <v>1023</v>
+        <v>53</v>
       </c>
     </row>
     <row r="498" spans="1:14" x14ac:dyDescent="0.25">
@@ -18513,7 +18513,7 @@
       </c>
       <c r="N500" s="15">
         <f t="shared" si="55"/>
-        <v>1023</v>
+        <v>44</v>
       </c>
     </row>
     <row r="501" spans="1:14" x14ac:dyDescent="0.25">
@@ -18627,7 +18627,7 @@
       </c>
       <c r="N503" s="15">
         <f t="shared" si="55"/>
-        <v>1023</v>
+        <v>35</v>
       </c>
     </row>
     <row r="504" spans="1:14" x14ac:dyDescent="0.25">
@@ -18741,7 +18741,7 @@
       </c>
       <c r="N506" s="15">
         <f t="shared" si="55"/>
-        <v>1024</v>
+        <v>25</v>
       </c>
     </row>
     <row r="507" spans="1:14" x14ac:dyDescent="0.25">
@@ -18855,7 +18855,7 @@
       </c>
       <c r="N509" s="15">
         <f t="shared" si="55"/>
-        <v>1024</v>
+        <v>16</v>
       </c>
     </row>
     <row r="510" spans="1:14" x14ac:dyDescent="0.25">
@@ -18969,7 +18969,7 @@
       </c>
       <c r="N512" s="15">
         <f t="shared" si="55"/>
-        <v>1024</v>
+        <v>6</v>
       </c>
     </row>
     <row r="513" spans="1:14" x14ac:dyDescent="0.25">
@@ -19077,8 +19077,8 @@
         <v>400</v>
       </c>
       <c r="N515" s="15">
-        <f t="shared" ref="N515:N578" si="64">IF((MOD(ROW(K515)-2,3)=0), K515, 9999)</f>
-        <v>1024</v>
+        <f t="shared" ref="N515:N578" si="64">IF((MOD(ROW(I515)-2,3)=0), I515, 9999)</f>
+        <v>-3</v>
       </c>
     </row>
     <row r="516" spans="1:14" x14ac:dyDescent="0.25">
@@ -19177,7 +19177,7 @@
       </c>
       <c r="N518" s="15">
         <f t="shared" si="64"/>
-        <v>1024</v>
+        <v>-13</v>
       </c>
     </row>
     <row r="519" spans="1:14" x14ac:dyDescent="0.25">
@@ -19276,7 +19276,7 @@
       </c>
       <c r="N521" s="15">
         <f t="shared" si="64"/>
-        <v>1024</v>
+        <v>-22</v>
       </c>
     </row>
     <row r="522" spans="1:14" x14ac:dyDescent="0.25">
@@ -19375,7 +19375,7 @@
       </c>
       <c r="N524" s="15">
         <f t="shared" si="64"/>
-        <v>1024</v>
+        <v>-31</v>
       </c>
     </row>
     <row r="525" spans="1:14" x14ac:dyDescent="0.25">
@@ -19474,7 +19474,7 @@
       </c>
       <c r="N527" s="15">
         <f t="shared" si="64"/>
-        <v>1023</v>
+        <v>-41</v>
       </c>
     </row>
     <row r="528" spans="1:14" x14ac:dyDescent="0.25">
@@ -19573,7 +19573,7 @@
       </c>
       <c r="N530" s="15">
         <f t="shared" si="64"/>
-        <v>1023</v>
+        <v>-50</v>
       </c>
     </row>
     <row r="531" spans="1:14" x14ac:dyDescent="0.25">
@@ -19672,7 +19672,7 @@
       </c>
       <c r="N533" s="15">
         <f t="shared" si="64"/>
-        <v>1022</v>
+        <v>-60</v>
       </c>
     </row>
     <row r="534" spans="1:14" x14ac:dyDescent="0.25">
@@ -19771,7 +19771,7 @@
       </c>
       <c r="N536" s="15">
         <f t="shared" si="64"/>
-        <v>1022</v>
+        <v>-69</v>
       </c>
     </row>
     <row r="537" spans="1:14" x14ac:dyDescent="0.25">
@@ -19870,7 +19870,7 @@
       </c>
       <c r="N539" s="15">
         <f t="shared" si="64"/>
-        <v>1021</v>
+        <v>-78</v>
       </c>
     </row>
     <row r="540" spans="1:14" x14ac:dyDescent="0.25">
@@ -19969,7 +19969,7 @@
       </c>
       <c r="N542" s="15">
         <f t="shared" si="64"/>
-        <v>1020</v>
+        <v>-88</v>
       </c>
     </row>
     <row r="543" spans="1:14" x14ac:dyDescent="0.25">
@@ -20068,7 +20068,7 @@
       </c>
       <c r="N545" s="15">
         <f t="shared" si="64"/>
-        <v>1019</v>
+        <v>-97</v>
       </c>
     </row>
     <row r="546" spans="1:14" x14ac:dyDescent="0.25">
@@ -20167,7 +20167,7 @@
       </c>
       <c r="N548" s="15">
         <f t="shared" si="64"/>
-        <v>1018</v>
+        <v>-107</v>
       </c>
     </row>
     <row r="549" spans="1:14" x14ac:dyDescent="0.25">
@@ -20266,7 +20266,7 @@
       </c>
       <c r="N551" s="15">
         <f t="shared" si="64"/>
-        <v>1017</v>
+        <v>-116</v>
       </c>
     </row>
     <row r="552" spans="1:14" x14ac:dyDescent="0.25">
@@ -20365,7 +20365,7 @@
       </c>
       <c r="N554" s="15">
         <f t="shared" si="64"/>
-        <v>1016</v>
+        <v>-125</v>
       </c>
     </row>
     <row r="555" spans="1:14" x14ac:dyDescent="0.25">
@@ -20464,7 +20464,7 @@
       </c>
       <c r="N557" s="15">
         <f t="shared" si="64"/>
-        <v>1015</v>
+        <v>-135</v>
       </c>
     </row>
     <row r="558" spans="1:14" x14ac:dyDescent="0.25">
@@ -20563,7 +20563,7 @@
       </c>
       <c r="N560" s="15">
         <f t="shared" si="64"/>
-        <v>1014</v>
+        <v>-144</v>
       </c>
     </row>
     <row r="561" spans="1:14" x14ac:dyDescent="0.25">
@@ -20662,7 +20662,7 @@
       </c>
       <c r="N563" s="15">
         <f t="shared" si="64"/>
-        <v>1012</v>
+        <v>-153</v>
       </c>
     </row>
     <row r="564" spans="1:14" x14ac:dyDescent="0.25">
@@ -20761,7 +20761,7 @@
       </c>
       <c r="N566" s="15">
         <f t="shared" si="64"/>
-        <v>1011</v>
+        <v>-163</v>
       </c>
     </row>
     <row r="567" spans="1:14" x14ac:dyDescent="0.25">
@@ -20860,7 +20860,7 @@
       </c>
       <c r="N569" s="15">
         <f t="shared" si="64"/>
-        <v>1009</v>
+        <v>-172</v>
       </c>
     </row>
     <row r="570" spans="1:14" x14ac:dyDescent="0.25">
@@ -20959,7 +20959,7 @@
       </c>
       <c r="N572" s="15">
         <f t="shared" si="64"/>
-        <v>1008</v>
+        <v>-181</v>
       </c>
     </row>
     <row r="573" spans="1:14" x14ac:dyDescent="0.25">
@@ -21058,7 +21058,7 @@
       </c>
       <c r="N575" s="15">
         <f t="shared" si="64"/>
-        <v>1006</v>
+        <v>-191</v>
       </c>
     </row>
     <row r="576" spans="1:14" x14ac:dyDescent="0.25">
@@ -21157,7 +21157,7 @@
       </c>
       <c r="N578" s="15">
         <f t="shared" si="64"/>
-        <v>1004</v>
+        <v>-200</v>
       </c>
     </row>
     <row r="579" spans="1:14" x14ac:dyDescent="0.25">
@@ -21189,7 +21189,7 @@
         <v>3EC</v>
       </c>
       <c r="N579" s="15">
-        <f t="shared" ref="N579:N642" si="71">IF((MOD(ROW(K579)-2,3)=0), K579, 9999)</f>
+        <f t="shared" ref="N579:N642" si="71">IF((MOD(ROW(I579)-2,3)=0), I579, 9999)</f>
         <v>9999</v>
       </c>
     </row>
@@ -21256,7 +21256,7 @@
       </c>
       <c r="N581" s="15">
         <f t="shared" si="71"/>
-        <v>1002</v>
+        <v>-209</v>
       </c>
     </row>
     <row r="582" spans="1:14" x14ac:dyDescent="0.25">
@@ -21355,7 +21355,7 @@
       </c>
       <c r="N584" s="15">
         <f t="shared" si="71"/>
-        <v>1000</v>
+        <v>-218</v>
       </c>
     </row>
     <row r="585" spans="1:14" x14ac:dyDescent="0.25">
@@ -21454,7 +21454,7 @@
       </c>
       <c r="N587" s="15">
         <f t="shared" si="71"/>
-        <v>998</v>
+        <v>-227</v>
       </c>
     </row>
     <row r="588" spans="1:14" x14ac:dyDescent="0.25">
@@ -21553,7 +21553,7 @@
       </c>
       <c r="N590" s="15">
         <f t="shared" si="71"/>
-        <v>996</v>
+        <v>-237</v>
       </c>
     </row>
     <row r="591" spans="1:14" x14ac:dyDescent="0.25">
@@ -21652,7 +21652,7 @@
       </c>
       <c r="N593" s="15">
         <f t="shared" si="71"/>
-        <v>994</v>
+        <v>-246</v>
       </c>
     </row>
     <row r="594" spans="1:14" x14ac:dyDescent="0.25">
@@ -21751,7 +21751,7 @@
       </c>
       <c r="N596" s="15">
         <f t="shared" si="71"/>
-        <v>992</v>
+        <v>-255</v>
       </c>
     </row>
     <row r="597" spans="1:14" x14ac:dyDescent="0.25">
@@ -21850,7 +21850,7 @@
       </c>
       <c r="N599" s="15">
         <f t="shared" si="71"/>
-        <v>989</v>
+        <v>-264</v>
       </c>
     </row>
     <row r="600" spans="1:14" x14ac:dyDescent="0.25">
@@ -21949,7 +21949,7 @@
       </c>
       <c r="N602" s="15">
         <f t="shared" si="71"/>
-        <v>987</v>
+        <v>-273</v>
       </c>
     </row>
     <row r="603" spans="1:14" x14ac:dyDescent="0.25">
@@ -22048,7 +22048,7 @@
       </c>
       <c r="N605" s="15">
         <f t="shared" si="71"/>
-        <v>984</v>
+        <v>-282</v>
       </c>
     </row>
     <row r="606" spans="1:14" x14ac:dyDescent="0.25">
@@ -22147,7 +22147,7 @@
       </c>
       <c r="N608" s="15">
         <f t="shared" si="71"/>
-        <v>982</v>
+        <v>-291</v>
       </c>
     </row>
     <row r="609" spans="1:14" x14ac:dyDescent="0.25">
@@ -22246,7 +22246,7 @@
       </c>
       <c r="N611" s="15">
         <f t="shared" si="71"/>
-        <v>979</v>
+        <v>-300</v>
       </c>
     </row>
     <row r="612" spans="1:14" x14ac:dyDescent="0.25">
@@ -22345,7 +22345,7 @@
       </c>
       <c r="N614" s="15">
         <f t="shared" si="71"/>
-        <v>976</v>
+        <v>-309</v>
       </c>
     </row>
     <row r="615" spans="1:14" x14ac:dyDescent="0.25">
@@ -22444,7 +22444,7 @@
       </c>
       <c r="N617" s="15">
         <f t="shared" si="71"/>
-        <v>973</v>
+        <v>-318</v>
       </c>
     </row>
     <row r="618" spans="1:14" x14ac:dyDescent="0.25">
@@ -22543,7 +22543,7 @@
       </c>
       <c r="N620" s="15">
         <f t="shared" si="71"/>
-        <v>970</v>
+        <v>-327</v>
       </c>
     </row>
     <row r="621" spans="1:14" x14ac:dyDescent="0.25">
@@ -22642,7 +22642,7 @@
       </c>
       <c r="N623" s="15">
         <f t="shared" si="71"/>
-        <v>967</v>
+        <v>-336</v>
       </c>
     </row>
     <row r="624" spans="1:14" x14ac:dyDescent="0.25">
@@ -22741,7 +22741,7 @@
       </c>
       <c r="N626" s="15">
         <f t="shared" si="71"/>
-        <v>964</v>
+        <v>-345</v>
       </c>
     </row>
     <row r="627" spans="1:14" x14ac:dyDescent="0.25">
@@ -22840,7 +22840,7 @@
       </c>
       <c r="N629" s="15">
         <f t="shared" si="71"/>
-        <v>961</v>
+        <v>-354</v>
       </c>
     </row>
     <row r="630" spans="1:14" x14ac:dyDescent="0.25">
@@ -22939,7 +22939,7 @@
       </c>
       <c r="N632" s="15">
         <f t="shared" si="71"/>
-        <v>958</v>
+        <v>-363</v>
       </c>
     </row>
     <row r="633" spans="1:14" x14ac:dyDescent="0.25">
@@ -23038,7 +23038,7 @@
       </c>
       <c r="N635" s="15">
         <f t="shared" si="71"/>
-        <v>954</v>
+        <v>-371</v>
       </c>
     </row>
     <row r="636" spans="1:14" x14ac:dyDescent="0.25">
@@ -23137,7 +23137,7 @@
       </c>
       <c r="N638" s="15">
         <f t="shared" si="71"/>
-        <v>951</v>
+        <v>-380</v>
       </c>
     </row>
     <row r="639" spans="1:14" x14ac:dyDescent="0.25">
@@ -23236,7 +23236,7 @@
       </c>
       <c r="N641" s="15">
         <f t="shared" si="71"/>
-        <v>947</v>
+        <v>-389</v>
       </c>
     </row>
     <row r="642" spans="1:14" x14ac:dyDescent="0.25">
@@ -23301,7 +23301,7 @@
         <v>3B1</v>
       </c>
       <c r="N643" s="15">
-        <f t="shared" ref="N643:N706" si="78">IF((MOD(ROW(K643)-2,3)=0), K643, 9999)</f>
+        <f t="shared" ref="N643:N706" si="78">IF((MOD(ROW(I643)-2,3)=0), I643, 9999)</f>
         <v>9999</v>
       </c>
     </row>
@@ -23335,7 +23335,7 @@
       </c>
       <c r="N644" s="15">
         <f t="shared" si="78"/>
-        <v>944</v>
+        <v>-398</v>
       </c>
     </row>
     <row r="645" spans="1:14" x14ac:dyDescent="0.25">
@@ -23434,7 +23434,7 @@
       </c>
       <c r="N647" s="15">
         <f t="shared" si="78"/>
-        <v>940</v>
+        <v>-406</v>
       </c>
     </row>
     <row r="648" spans="1:14" x14ac:dyDescent="0.25">
@@ -23533,7 +23533,7 @@
       </c>
       <c r="N650" s="15">
         <f t="shared" si="78"/>
-        <v>936</v>
+        <v>-415</v>
       </c>
     </row>
     <row r="651" spans="1:14" x14ac:dyDescent="0.25">
@@ -23632,7 +23632,7 @@
       </c>
       <c r="N653" s="15">
         <f t="shared" si="78"/>
-        <v>932</v>
+        <v>-424</v>
       </c>
     </row>
     <row r="654" spans="1:14" x14ac:dyDescent="0.25">
@@ -23731,7 +23731,7 @@
       </c>
       <c r="N656" s="15">
         <f t="shared" si="78"/>
-        <v>928</v>
+        <v>-432</v>
       </c>
     </row>
     <row r="657" spans="1:14" x14ac:dyDescent="0.25">
@@ -23830,7 +23830,7 @@
       </c>
       <c r="N659" s="15">
         <f t="shared" si="78"/>
-        <v>924</v>
+        <v>-441</v>
       </c>
     </row>
     <row r="660" spans="1:14" x14ac:dyDescent="0.25">
@@ -23929,7 +23929,7 @@
       </c>
       <c r="N662" s="15">
         <f t="shared" si="78"/>
-        <v>920</v>
+        <v>-449</v>
       </c>
     </row>
     <row r="663" spans="1:14" x14ac:dyDescent="0.25">
@@ -24028,7 +24028,7 @@
       </c>
       <c r="N665" s="15">
         <f t="shared" si="78"/>
-        <v>916</v>
+        <v>-458</v>
       </c>
     </row>
     <row r="666" spans="1:14" x14ac:dyDescent="0.25">
@@ -24127,7 +24127,7 @@
       </c>
       <c r="N668" s="15">
         <f t="shared" si="78"/>
-        <v>912</v>
+        <v>-466</v>
       </c>
     </row>
     <row r="669" spans="1:14" x14ac:dyDescent="0.25">
@@ -24226,7 +24226,7 @@
       </c>
       <c r="N671" s="15">
         <f t="shared" si="78"/>
-        <v>907</v>
+        <v>-474</v>
       </c>
     </row>
     <row r="672" spans="1:14" x14ac:dyDescent="0.25">
@@ -24325,7 +24325,7 @@
       </c>
       <c r="N674" s="15">
         <f t="shared" si="78"/>
-        <v>903</v>
+        <v>-483</v>
       </c>
     </row>
     <row r="675" spans="1:14" x14ac:dyDescent="0.25">
@@ -24424,7 +24424,7 @@
       </c>
       <c r="N677" s="15">
         <f t="shared" si="78"/>
-        <v>899</v>
+        <v>-491</v>
       </c>
     </row>
     <row r="678" spans="1:14" x14ac:dyDescent="0.25">
@@ -24523,7 +24523,7 @@
       </c>
       <c r="N680" s="15">
         <f t="shared" si="78"/>
-        <v>894</v>
+        <v>-499</v>
       </c>
     </row>
     <row r="681" spans="1:14" x14ac:dyDescent="0.25">
@@ -24622,7 +24622,7 @@
       </c>
       <c r="N683" s="15">
         <f t="shared" si="78"/>
-        <v>889</v>
+        <v>-507</v>
       </c>
     </row>
     <row r="684" spans="1:14" x14ac:dyDescent="0.25">
@@ -24721,7 +24721,7 @@
       </c>
       <c r="N686" s="15">
         <f t="shared" si="78"/>
-        <v>885</v>
+        <v>-516</v>
       </c>
     </row>
     <row r="687" spans="1:14" x14ac:dyDescent="0.25">
@@ -24820,7 +24820,7 @@
       </c>
       <c r="N689" s="15">
         <f t="shared" si="78"/>
-        <v>880</v>
+        <v>-524</v>
       </c>
     </row>
     <row r="690" spans="1:14" x14ac:dyDescent="0.25">
@@ -24919,7 +24919,7 @@
       </c>
       <c r="N692" s="15">
         <f t="shared" si="78"/>
-        <v>875</v>
+        <v>-532</v>
       </c>
     </row>
     <row r="693" spans="1:14" x14ac:dyDescent="0.25">
@@ -25018,7 +25018,7 @@
       </c>
       <c r="N695" s="15">
         <f t="shared" si="78"/>
-        <v>870</v>
+        <v>-540</v>
       </c>
     </row>
     <row r="696" spans="1:14" x14ac:dyDescent="0.25">
@@ -25117,7 +25117,7 @@
       </c>
       <c r="N698" s="15">
         <f t="shared" si="78"/>
-        <v>865</v>
+        <v>-548</v>
       </c>
     </row>
     <row r="699" spans="1:14" x14ac:dyDescent="0.25">
@@ -25216,7 +25216,7 @@
       </c>
       <c r="N701" s="15">
         <f t="shared" si="78"/>
-        <v>860</v>
+        <v>-556</v>
       </c>
     </row>
     <row r="702" spans="1:14" x14ac:dyDescent="0.25">
@@ -25315,7 +25315,7 @@
       </c>
       <c r="N704" s="15">
         <f t="shared" si="78"/>
-        <v>855</v>
+        <v>-564</v>
       </c>
     </row>
     <row r="705" spans="1:14" x14ac:dyDescent="0.25">
@@ -25413,8 +25413,8 @@
         <v>352</v>
       </c>
       <c r="N707" s="15">
-        <f t="shared" ref="N707:N770" si="85">IF((MOD(ROW(K707)-2,3)=0), K707, 9999)</f>
-        <v>850</v>
+        <f t="shared" ref="N707:N770" si="85">IF((MOD(ROW(I707)-2,3)=0), I707, 9999)</f>
+        <v>-572</v>
       </c>
     </row>
     <row r="708" spans="1:14" x14ac:dyDescent="0.25">
@@ -25513,7 +25513,7 @@
       </c>
       <c r="N710" s="15">
         <f t="shared" si="85"/>
-        <v>844</v>
+        <v>-579</v>
       </c>
     </row>
     <row r="711" spans="1:14" x14ac:dyDescent="0.25">
@@ -25612,7 +25612,7 @@
       </c>
       <c r="N713" s="15">
         <f t="shared" si="85"/>
-        <v>839</v>
+        <v>-587</v>
       </c>
     </row>
     <row r="714" spans="1:14" x14ac:dyDescent="0.25">
@@ -25711,7 +25711,7 @@
       </c>
       <c r="N716" s="15">
         <f t="shared" si="85"/>
-        <v>834</v>
+        <v>-595</v>
       </c>
     </row>
     <row r="717" spans="1:14" x14ac:dyDescent="0.25">
@@ -25810,7 +25810,7 @@
       </c>
       <c r="N719" s="15">
         <f t="shared" si="85"/>
-        <v>828</v>
+        <v>-602</v>
       </c>
     </row>
     <row r="720" spans="1:14" x14ac:dyDescent="0.25">
@@ -25909,7 +25909,7 @@
       </c>
       <c r="N722" s="15">
         <f t="shared" si="85"/>
-        <v>822</v>
+        <v>-610</v>
       </c>
     </row>
     <row r="723" spans="1:14" x14ac:dyDescent="0.25">
@@ -26008,7 +26008,7 @@
       </c>
       <c r="N725" s="15">
         <f t="shared" si="85"/>
-        <v>817</v>
+        <v>-618</v>
       </c>
     </row>
     <row r="726" spans="1:14" x14ac:dyDescent="0.25">
@@ -26107,7 +26107,7 @@
       </c>
       <c r="N728" s="15">
         <f t="shared" si="85"/>
-        <v>811</v>
+        <v>-625</v>
       </c>
     </row>
     <row r="729" spans="1:14" x14ac:dyDescent="0.25">
@@ -26206,7 +26206,7 @@
       </c>
       <c r="N731" s="15">
         <f t="shared" si="85"/>
-        <v>805</v>
+        <v>-632</v>
       </c>
     </row>
     <row r="732" spans="1:14" x14ac:dyDescent="0.25">
@@ -26305,7 +26305,7 @@
       </c>
       <c r="N734" s="15">
         <f t="shared" si="85"/>
-        <v>799</v>
+        <v>-640</v>
       </c>
     </row>
     <row r="735" spans="1:14" x14ac:dyDescent="0.25">
@@ -26404,7 +26404,7 @@
       </c>
       <c r="N737" s="15">
         <f t="shared" si="85"/>
-        <v>794</v>
+        <v>-647</v>
       </c>
     </row>
     <row r="738" spans="1:14" x14ac:dyDescent="0.25">
@@ -26503,7 +26503,7 @@
       </c>
       <c r="N740" s="15">
         <f t="shared" si="85"/>
-        <v>788</v>
+        <v>-654</v>
       </c>
     </row>
     <row r="741" spans="1:14" x14ac:dyDescent="0.25">
@@ -26602,7 +26602,7 @@
       </c>
       <c r="N743" s="15">
         <f t="shared" si="85"/>
-        <v>782</v>
+        <v>-662</v>
       </c>
     </row>
     <row r="744" spans="1:14" x14ac:dyDescent="0.25">
@@ -26701,7 +26701,7 @@
       </c>
       <c r="N746" s="15">
         <f t="shared" si="85"/>
-        <v>775</v>
+        <v>-669</v>
       </c>
     </row>
     <row r="747" spans="1:14" x14ac:dyDescent="0.25">
@@ -26800,7 +26800,7 @@
       </c>
       <c r="N749" s="15">
         <f t="shared" si="85"/>
-        <v>769</v>
+        <v>-676</v>
       </c>
     </row>
     <row r="750" spans="1:14" x14ac:dyDescent="0.25">
@@ -26899,7 +26899,7 @@
       </c>
       <c r="N752" s="15">
         <f t="shared" si="85"/>
-        <v>763</v>
+        <v>-683</v>
       </c>
     </row>
     <row r="753" spans="1:14" x14ac:dyDescent="0.25">
@@ -26998,7 +26998,7 @@
       </c>
       <c r="N755" s="15">
         <f t="shared" si="85"/>
-        <v>757</v>
+        <v>-690</v>
       </c>
     </row>
     <row r="756" spans="1:14" x14ac:dyDescent="0.25">
@@ -27097,7 +27097,7 @@
       </c>
       <c r="N758" s="15">
         <f t="shared" si="85"/>
-        <v>750</v>
+        <v>-697</v>
       </c>
     </row>
     <row r="759" spans="1:14" x14ac:dyDescent="0.25">
@@ -27196,7 +27196,7 @@
       </c>
       <c r="N761" s="15">
         <f t="shared" si="85"/>
-        <v>744</v>
+        <v>-704</v>
       </c>
     </row>
     <row r="762" spans="1:14" x14ac:dyDescent="0.25">
@@ -27295,7 +27295,7 @@
       </c>
       <c r="N764" s="15">
         <f t="shared" si="85"/>
-        <v>737</v>
+        <v>-711</v>
       </c>
     </row>
     <row r="765" spans="1:14" x14ac:dyDescent="0.25">
@@ -27394,7 +27394,7 @@
       </c>
       <c r="N767" s="15">
         <f t="shared" si="85"/>
-        <v>731</v>
+        <v>-717</v>
       </c>
     </row>
     <row r="768" spans="1:14" x14ac:dyDescent="0.25">
@@ -27493,7 +27493,7 @@
       </c>
       <c r="N770" s="15">
         <f t="shared" si="85"/>
-        <v>724</v>
+        <v>-724</v>
       </c>
     </row>
     <row r="771" spans="1:14" x14ac:dyDescent="0.25">
@@ -27525,7 +27525,7 @@
         <v>2D2</v>
       </c>
       <c r="N771" s="15">
-        <f t="shared" ref="N771:N834" si="92">IF((MOD(ROW(K771)-2,3)=0), K771, 9999)</f>
+        <f t="shared" ref="N771:N834" si="92">IF((MOD(ROW(I771)-2,3)=0), I771, 9999)</f>
         <v>9999</v>
       </c>
     </row>
@@ -27592,7 +27592,7 @@
       </c>
       <c r="N773" s="15">
         <f t="shared" si="92"/>
-        <v>717</v>
+        <v>-731</v>
       </c>
     </row>
     <row r="774" spans="1:14" x14ac:dyDescent="0.25">
@@ -27691,7 +27691,7 @@
       </c>
       <c r="N776" s="15">
         <f t="shared" si="92"/>
-        <v>711</v>
+        <v>-737</v>
       </c>
     </row>
     <row r="777" spans="1:14" x14ac:dyDescent="0.25">
@@ -27790,7 +27790,7 @@
       </c>
       <c r="N779" s="15">
         <f t="shared" si="92"/>
-        <v>704</v>
+        <v>-744</v>
       </c>
     </row>
     <row r="780" spans="1:14" x14ac:dyDescent="0.25">
@@ -27889,7 +27889,7 @@
       </c>
       <c r="N782" s="15">
         <f t="shared" si="92"/>
-        <v>697</v>
+        <v>-750</v>
       </c>
     </row>
     <row r="783" spans="1:14" x14ac:dyDescent="0.25">
@@ -27988,7 +27988,7 @@
       </c>
       <c r="N785" s="15">
         <f t="shared" si="92"/>
-        <v>690</v>
+        <v>-757</v>
       </c>
     </row>
     <row r="786" spans="1:14" x14ac:dyDescent="0.25">
@@ -28087,7 +28087,7 @@
       </c>
       <c r="N788" s="15">
         <f t="shared" si="92"/>
-        <v>683</v>
+        <v>-763</v>
       </c>
     </row>
     <row r="789" spans="1:14" x14ac:dyDescent="0.25">
@@ -28186,7 +28186,7 @@
       </c>
       <c r="N791" s="15">
         <f t="shared" si="92"/>
-        <v>676</v>
+        <v>-769</v>
       </c>
     </row>
     <row r="792" spans="1:14" x14ac:dyDescent="0.25">
@@ -28285,7 +28285,7 @@
       </c>
       <c r="N794" s="15">
         <f t="shared" si="92"/>
-        <v>669</v>
+        <v>-775</v>
       </c>
     </row>
     <row r="795" spans="1:14" x14ac:dyDescent="0.25">
@@ -28384,7 +28384,7 @@
       </c>
       <c r="N797" s="15">
         <f t="shared" si="92"/>
-        <v>662</v>
+        <v>-782</v>
       </c>
     </row>
     <row r="798" spans="1:14" x14ac:dyDescent="0.25">
@@ -28483,7 +28483,7 @@
       </c>
       <c r="N800" s="15">
         <f t="shared" si="92"/>
-        <v>654</v>
+        <v>-788</v>
       </c>
     </row>
     <row r="801" spans="1:14" x14ac:dyDescent="0.25">
@@ -28582,7 +28582,7 @@
       </c>
       <c r="N803" s="15">
         <f t="shared" si="92"/>
-        <v>647</v>
+        <v>-794</v>
       </c>
     </row>
     <row r="804" spans="1:14" x14ac:dyDescent="0.25">
@@ -28681,7 +28681,7 @@
       </c>
       <c r="N806" s="15">
         <f t="shared" si="92"/>
-        <v>640</v>
+        <v>-799</v>
       </c>
     </row>
     <row r="807" spans="1:14" x14ac:dyDescent="0.25">
@@ -28780,7 +28780,7 @@
       </c>
       <c r="N809" s="15">
         <f t="shared" si="92"/>
-        <v>632</v>
+        <v>-805</v>
       </c>
     </row>
     <row r="810" spans="1:14" x14ac:dyDescent="0.25">
@@ -28879,7 +28879,7 @@
       </c>
       <c r="N812" s="15">
         <f t="shared" si="92"/>
-        <v>625</v>
+        <v>-811</v>
       </c>
     </row>
     <row r="813" spans="1:14" x14ac:dyDescent="0.25">
@@ -28978,7 +28978,7 @@
       </c>
       <c r="N815" s="15">
         <f t="shared" si="92"/>
-        <v>618</v>
+        <v>-817</v>
       </c>
     </row>
     <row r="816" spans="1:14" x14ac:dyDescent="0.25">
@@ -29077,7 +29077,7 @@
       </c>
       <c r="N818" s="15">
         <f t="shared" si="92"/>
-        <v>610</v>
+        <v>-822</v>
       </c>
     </row>
     <row r="819" spans="1:14" x14ac:dyDescent="0.25">
@@ -29176,7 +29176,7 @@
       </c>
       <c r="N821" s="15">
         <f t="shared" si="92"/>
-        <v>602</v>
+        <v>-828</v>
       </c>
     </row>
     <row r="822" spans="1:14" x14ac:dyDescent="0.25">
@@ -29275,7 +29275,7 @@
       </c>
       <c r="N824" s="15">
         <f t="shared" si="92"/>
-        <v>595</v>
+        <v>-834</v>
       </c>
     </row>
     <row r="825" spans="1:14" x14ac:dyDescent="0.25">
@@ -29374,7 +29374,7 @@
       </c>
       <c r="N827" s="15">
         <f t="shared" si="92"/>
-        <v>587</v>
+        <v>-839</v>
       </c>
     </row>
     <row r="828" spans="1:14" x14ac:dyDescent="0.25">
@@ -29473,7 +29473,7 @@
       </c>
       <c r="N830" s="15">
         <f t="shared" si="92"/>
-        <v>579</v>
+        <v>-844</v>
       </c>
     </row>
     <row r="831" spans="1:14" x14ac:dyDescent="0.25">
@@ -29572,7 +29572,7 @@
       </c>
       <c r="N833" s="15">
         <f t="shared" si="92"/>
-        <v>572</v>
+        <v>-850</v>
       </c>
     </row>
     <row r="834" spans="1:14" x14ac:dyDescent="0.25">
@@ -29637,7 +29637,7 @@
         <v>236</v>
       </c>
       <c r="N835" s="15">
-        <f t="shared" ref="N835:N898" si="99">IF((MOD(ROW(K835)-2,3)=0), K835, 9999)</f>
+        <f t="shared" ref="N835:N898" si="99">IF((MOD(ROW(I835)-2,3)=0), I835, 9999)</f>
         <v>9999</v>
       </c>
     </row>
@@ -29671,7 +29671,7 @@
       </c>
       <c r="N836" s="15">
         <f t="shared" si="99"/>
-        <v>564</v>
+        <v>-855</v>
       </c>
     </row>
     <row r="837" spans="1:14" x14ac:dyDescent="0.25">
@@ -29770,7 +29770,7 @@
       </c>
       <c r="N839" s="15">
         <f t="shared" si="99"/>
-        <v>556</v>
+        <v>-860</v>
       </c>
     </row>
     <row r="840" spans="1:14" x14ac:dyDescent="0.25">
@@ -29869,7 +29869,7 @@
       </c>
       <c r="N842" s="15">
         <f t="shared" si="99"/>
-        <v>548</v>
+        <v>-865</v>
       </c>
     </row>
     <row r="843" spans="1:14" x14ac:dyDescent="0.25">
@@ -29968,7 +29968,7 @@
       </c>
       <c r="N845" s="15">
         <f t="shared" si="99"/>
-        <v>540</v>
+        <v>-870</v>
       </c>
     </row>
     <row r="846" spans="1:14" x14ac:dyDescent="0.25">
@@ -30067,7 +30067,7 @@
       </c>
       <c r="N848" s="15">
         <f t="shared" si="99"/>
-        <v>532</v>
+        <v>-875</v>
       </c>
     </row>
     <row r="849" spans="1:14" x14ac:dyDescent="0.25">
@@ -30166,7 +30166,7 @@
       </c>
       <c r="N851" s="15">
         <f t="shared" si="99"/>
-        <v>524</v>
+        <v>-880</v>
       </c>
     </row>
     <row r="852" spans="1:14" x14ac:dyDescent="0.25">
@@ -30265,7 +30265,7 @@
       </c>
       <c r="N854" s="15">
         <f t="shared" si="99"/>
-        <v>516</v>
+        <v>-885</v>
       </c>
     </row>
     <row r="855" spans="1:14" x14ac:dyDescent="0.25">
@@ -30364,7 +30364,7 @@
       </c>
       <c r="N857" s="15">
         <f t="shared" si="99"/>
-        <v>507</v>
+        <v>-889</v>
       </c>
     </row>
     <row r="858" spans="1:14" x14ac:dyDescent="0.25">
@@ -30463,7 +30463,7 @@
       </c>
       <c r="N860" s="15">
         <f t="shared" si="99"/>
-        <v>499</v>
+        <v>-894</v>
       </c>
     </row>
     <row r="861" spans="1:14" x14ac:dyDescent="0.25">
@@ -30562,7 +30562,7 @@
       </c>
       <c r="N863" s="15">
         <f t="shared" si="99"/>
-        <v>491</v>
+        <v>-899</v>
       </c>
     </row>
     <row r="864" spans="1:14" x14ac:dyDescent="0.25">
@@ -30661,7 +30661,7 @@
       </c>
       <c r="N866" s="15">
         <f t="shared" si="99"/>
-        <v>483</v>
+        <v>-903</v>
       </c>
     </row>
     <row r="867" spans="1:14" x14ac:dyDescent="0.25">
@@ -30760,7 +30760,7 @@
       </c>
       <c r="N869" s="15">
         <f t="shared" si="99"/>
-        <v>474</v>
+        <v>-907</v>
       </c>
     </row>
     <row r="870" spans="1:14" x14ac:dyDescent="0.25">
@@ -30859,7 +30859,7 @@
       </c>
       <c r="N872" s="15">
         <f t="shared" si="99"/>
-        <v>466</v>
+        <v>-912</v>
       </c>
     </row>
     <row r="873" spans="1:14" x14ac:dyDescent="0.25">
@@ -30958,7 +30958,7 @@
       </c>
       <c r="N875" s="15">
         <f t="shared" si="99"/>
-        <v>458</v>
+        <v>-916</v>
       </c>
     </row>
     <row r="876" spans="1:14" x14ac:dyDescent="0.25">
@@ -31057,7 +31057,7 @@
       </c>
       <c r="N878" s="15">
         <f t="shared" si="99"/>
-        <v>449</v>
+        <v>-920</v>
       </c>
     </row>
     <row r="879" spans="1:14" x14ac:dyDescent="0.25">
@@ -31156,7 +31156,7 @@
       </c>
       <c r="N881" s="15">
         <f t="shared" si="99"/>
-        <v>441</v>
+        <v>-924</v>
       </c>
     </row>
     <row r="882" spans="1:14" x14ac:dyDescent="0.25">
@@ -31255,7 +31255,7 @@
       </c>
       <c r="N884" s="15">
         <f t="shared" si="99"/>
-        <v>432</v>
+        <v>-928</v>
       </c>
     </row>
     <row r="885" spans="1:14" x14ac:dyDescent="0.25">
@@ -31354,7 +31354,7 @@
       </c>
       <c r="N887" s="15">
         <f t="shared" si="99"/>
-        <v>424</v>
+        <v>-932</v>
       </c>
     </row>
     <row r="888" spans="1:14" x14ac:dyDescent="0.25">
@@ -31453,7 +31453,7 @@
       </c>
       <c r="N890" s="15">
         <f t="shared" si="99"/>
-        <v>415</v>
+        <v>-936</v>
       </c>
     </row>
     <row r="891" spans="1:14" x14ac:dyDescent="0.25">
@@ -31552,7 +31552,7 @@
       </c>
       <c r="N893" s="15">
         <f t="shared" si="99"/>
-        <v>406</v>
+        <v>-940</v>
       </c>
     </row>
     <row r="894" spans="1:14" x14ac:dyDescent="0.25">
@@ -31651,7 +31651,7 @@
       </c>
       <c r="N896" s="15">
         <f t="shared" si="99"/>
-        <v>398</v>
+        <v>-944</v>
       </c>
     </row>
     <row r="897" spans="1:14" x14ac:dyDescent="0.25">
@@ -31749,8 +31749,8 @@
         <v>185</v>
       </c>
       <c r="N899" s="15">
-        <f t="shared" ref="N899:N962" si="106">IF((MOD(ROW(K899)-2,3)=0), K899, 9999)</f>
-        <v>389</v>
+        <f t="shared" ref="N899:N962" si="106">IF((MOD(ROW(I899)-2,3)=0), I899, 9999)</f>
+        <v>-947</v>
       </c>
     </row>
     <row r="900" spans="1:14" x14ac:dyDescent="0.25">
@@ -31849,7 +31849,7 @@
       </c>
       <c r="N902" s="15">
         <f t="shared" si="106"/>
-        <v>380</v>
+        <v>-951</v>
       </c>
     </row>
     <row r="903" spans="1:14" x14ac:dyDescent="0.25">
@@ -31948,7 +31948,7 @@
       </c>
       <c r="N905" s="15">
         <f t="shared" si="106"/>
-        <v>371</v>
+        <v>-954</v>
       </c>
     </row>
     <row r="906" spans="1:14" x14ac:dyDescent="0.25">
@@ -32047,7 +32047,7 @@
       </c>
       <c r="N908" s="15">
         <f t="shared" si="106"/>
-        <v>363</v>
+        <v>-958</v>
       </c>
     </row>
     <row r="909" spans="1:14" x14ac:dyDescent="0.25">
@@ -32146,7 +32146,7 @@
       </c>
       <c r="N911" s="15">
         <f t="shared" si="106"/>
-        <v>354</v>
+        <v>-961</v>
       </c>
     </row>
     <row r="912" spans="1:14" x14ac:dyDescent="0.25">
@@ -32245,7 +32245,7 @@
       </c>
       <c r="N914" s="15">
         <f t="shared" si="106"/>
-        <v>345</v>
+        <v>-964</v>
       </c>
     </row>
     <row r="915" spans="1:14" x14ac:dyDescent="0.25">
@@ -32344,7 +32344,7 @@
       </c>
       <c r="N917" s="15">
         <f t="shared" si="106"/>
-        <v>336</v>
+        <v>-967</v>
       </c>
     </row>
     <row r="918" spans="1:14" x14ac:dyDescent="0.25">
@@ -32443,7 +32443,7 @@
       </c>
       <c r="N920" s="15">
         <f t="shared" si="106"/>
-        <v>327</v>
+        <v>-970</v>
       </c>
     </row>
     <row r="921" spans="1:14" x14ac:dyDescent="0.25">
@@ -32542,7 +32542,7 @@
       </c>
       <c r="N923" s="15">
         <f t="shared" si="106"/>
-        <v>318</v>
+        <v>-973</v>
       </c>
     </row>
     <row r="924" spans="1:14" x14ac:dyDescent="0.25">
@@ -32641,7 +32641,7 @@
       </c>
       <c r="N926" s="15">
         <f t="shared" si="106"/>
-        <v>309</v>
+        <v>-976</v>
       </c>
     </row>
     <row r="927" spans="1:14" x14ac:dyDescent="0.25">
@@ -32740,7 +32740,7 @@
       </c>
       <c r="N929" s="15">
         <f t="shared" si="106"/>
-        <v>300</v>
+        <v>-979</v>
       </c>
     </row>
     <row r="930" spans="1:14" x14ac:dyDescent="0.25">
@@ -32839,7 +32839,7 @@
       </c>
       <c r="N932" s="15">
         <f t="shared" si="106"/>
-        <v>291</v>
+        <v>-982</v>
       </c>
     </row>
     <row r="933" spans="1:14" x14ac:dyDescent="0.25">
@@ -32938,7 +32938,7 @@
       </c>
       <c r="N935" s="15">
         <f t="shared" si="106"/>
-        <v>282</v>
+        <v>-984</v>
       </c>
     </row>
     <row r="936" spans="1:14" x14ac:dyDescent="0.25">
@@ -33037,7 +33037,7 @@
       </c>
       <c r="N938" s="15">
         <f t="shared" si="106"/>
-        <v>273</v>
+        <v>-987</v>
       </c>
     </row>
     <row r="939" spans="1:14" x14ac:dyDescent="0.25">
@@ -33136,7 +33136,7 @@
       </c>
       <c r="N941" s="15">
         <f t="shared" si="106"/>
-        <v>264</v>
+        <v>-989</v>
       </c>
     </row>
     <row r="942" spans="1:14" x14ac:dyDescent="0.25">
@@ -33235,7 +33235,7 @@
       </c>
       <c r="N944" s="15">
         <f t="shared" si="106"/>
-        <v>255</v>
+        <v>-992</v>
       </c>
     </row>
     <row r="945" spans="1:14" x14ac:dyDescent="0.25">
@@ -33334,7 +33334,7 @@
       </c>
       <c r="N947" s="15">
         <f t="shared" si="106"/>
-        <v>246</v>
+        <v>-994</v>
       </c>
     </row>
     <row r="948" spans="1:14" x14ac:dyDescent="0.25">
@@ -33433,7 +33433,7 @@
       </c>
       <c r="N950" s="15">
         <f t="shared" si="106"/>
-        <v>237</v>
+        <v>-996</v>
       </c>
     </row>
     <row r="951" spans="1:14" x14ac:dyDescent="0.25">
@@ -33532,7 +33532,7 @@
       </c>
       <c r="N953" s="15">
         <f t="shared" si="106"/>
-        <v>227</v>
+        <v>-998</v>
       </c>
     </row>
     <row r="954" spans="1:14" x14ac:dyDescent="0.25">
@@ -33631,7 +33631,7 @@
       </c>
       <c r="N956" s="15">
         <f t="shared" si="106"/>
-        <v>218</v>
+        <v>-1000</v>
       </c>
     </row>
     <row r="957" spans="1:14" x14ac:dyDescent="0.25">
@@ -33730,7 +33730,7 @@
       </c>
       <c r="N959" s="15">
         <f t="shared" si="106"/>
-        <v>209</v>
+        <v>-1002</v>
       </c>
     </row>
     <row r="960" spans="1:14" x14ac:dyDescent="0.25">
@@ -33829,7 +33829,7 @@
       </c>
       <c r="N962" s="15">
         <f t="shared" si="106"/>
-        <v>200</v>
+        <v>-1004</v>
       </c>
     </row>
     <row r="963" spans="1:14" x14ac:dyDescent="0.25">
@@ -33861,7 +33861,7 @@
         <v>0C5</v>
       </c>
       <c r="N963" s="15">
-        <f t="shared" ref="N963:N1026" si="113">IF((MOD(ROW(K963)-2,3)=0), K963, 9999)</f>
+        <f t="shared" ref="N963:N1026" si="113">IF((MOD(ROW(I963)-2,3)=0), I963, 9999)</f>
         <v>9999</v>
       </c>
     </row>
@@ -33928,7 +33928,7 @@
       </c>
       <c r="N965" s="15">
         <f t="shared" si="113"/>
-        <v>191</v>
+        <v>-1006</v>
       </c>
     </row>
     <row r="966" spans="1:14" x14ac:dyDescent="0.25">
@@ -34027,7 +34027,7 @@
       </c>
       <c r="N968" s="15">
         <f t="shared" si="113"/>
-        <v>181</v>
+        <v>-1008</v>
       </c>
     </row>
     <row r="969" spans="1:14" x14ac:dyDescent="0.25">
@@ -34126,7 +34126,7 @@
       </c>
       <c r="N971" s="15">
         <f t="shared" si="113"/>
-        <v>172</v>
+        <v>-1009</v>
       </c>
     </row>
     <row r="972" spans="1:14" x14ac:dyDescent="0.25">
@@ -34225,7 +34225,7 @@
       </c>
       <c r="N974" s="15">
         <f t="shared" si="113"/>
-        <v>163</v>
+        <v>-1011</v>
       </c>
     </row>
     <row r="975" spans="1:14" x14ac:dyDescent="0.25">
@@ -34324,7 +34324,7 @@
       </c>
       <c r="N977" s="15">
         <f t="shared" si="113"/>
-        <v>153</v>
+        <v>-1012</v>
       </c>
     </row>
     <row r="978" spans="1:14" x14ac:dyDescent="0.25">
@@ -34423,7 +34423,7 @@
       </c>
       <c r="N980" s="15">
         <f t="shared" si="113"/>
-        <v>144</v>
+        <v>-1014</v>
       </c>
     </row>
     <row r="981" spans="1:14" x14ac:dyDescent="0.25">
@@ -34522,7 +34522,7 @@
       </c>
       <c r="N983" s="15">
         <f t="shared" si="113"/>
-        <v>135</v>
+        <v>-1015</v>
       </c>
     </row>
     <row r="984" spans="1:14" x14ac:dyDescent="0.25">
@@ -34621,7 +34621,7 @@
       </c>
       <c r="N986" s="15">
         <f t="shared" si="113"/>
-        <v>125</v>
+        <v>-1016</v>
       </c>
     </row>
     <row r="987" spans="1:14" x14ac:dyDescent="0.25">
@@ -34720,7 +34720,7 @@
       </c>
       <c r="N989" s="15">
         <f t="shared" si="113"/>
-        <v>116</v>
+        <v>-1017</v>
       </c>
     </row>
     <row r="990" spans="1:14" x14ac:dyDescent="0.25">
@@ -34819,7 +34819,7 @@
       </c>
       <c r="N992" s="15">
         <f t="shared" si="113"/>
-        <v>107</v>
+        <v>-1018</v>
       </c>
     </row>
     <row r="993" spans="1:14" x14ac:dyDescent="0.25">
@@ -34918,7 +34918,7 @@
       </c>
       <c r="N995" s="15">
         <f t="shared" si="113"/>
-        <v>97</v>
+        <v>-1019</v>
       </c>
     </row>
     <row r="996" spans="1:14" x14ac:dyDescent="0.25">
@@ -35017,7 +35017,7 @@
       </c>
       <c r="N998" s="15">
         <f t="shared" si="113"/>
-        <v>88</v>
+        <v>-1020</v>
       </c>
     </row>
     <row r="999" spans="1:14" x14ac:dyDescent="0.25">
@@ -35116,7 +35116,7 @@
       </c>
       <c r="N1001" s="15">
         <f t="shared" si="113"/>
-        <v>78</v>
+        <v>-1021</v>
       </c>
     </row>
     <row r="1002" spans="1:14" x14ac:dyDescent="0.25">
@@ -35215,7 +35215,7 @@
       </c>
       <c r="N1004" s="15">
         <f t="shared" si="113"/>
-        <v>69</v>
+        <v>-1022</v>
       </c>
     </row>
     <row r="1005" spans="1:14" x14ac:dyDescent="0.25">
@@ -35314,7 +35314,7 @@
       </c>
       <c r="N1007" s="15">
         <f t="shared" si="113"/>
-        <v>60</v>
+        <v>-1022</v>
       </c>
     </row>
     <row r="1008" spans="1:14" x14ac:dyDescent="0.25">
@@ -35413,7 +35413,7 @@
       </c>
       <c r="N1010" s="15">
         <f t="shared" si="113"/>
-        <v>50</v>
+        <v>-1023</v>
       </c>
     </row>
     <row r="1011" spans="1:14" x14ac:dyDescent="0.25">
@@ -35512,7 +35512,7 @@
       </c>
       <c r="N1013" s="15">
         <f t="shared" si="113"/>
-        <v>41</v>
+        <v>-1023</v>
       </c>
     </row>
     <row r="1014" spans="1:14" x14ac:dyDescent="0.25">
@@ -35611,7 +35611,7 @@
       </c>
       <c r="N1016" s="15">
         <f t="shared" si="113"/>
-        <v>31</v>
+        <v>-1024</v>
       </c>
     </row>
     <row r="1017" spans="1:14" x14ac:dyDescent="0.25">
@@ -35710,7 +35710,7 @@
       </c>
       <c r="N1019" s="15">
         <f t="shared" si="113"/>
-        <v>22</v>
+        <v>-1024</v>
       </c>
     </row>
     <row r="1020" spans="1:14" x14ac:dyDescent="0.25">
@@ -35809,7 +35809,7 @@
       </c>
       <c r="N1022" s="15">
         <f t="shared" si="113"/>
-        <v>13</v>
+        <v>-1024</v>
       </c>
     </row>
     <row r="1023" spans="1:14" x14ac:dyDescent="0.25">
@@ -35908,7 +35908,7 @@
       </c>
       <c r="N1025" s="15">
         <f t="shared" si="113"/>
-        <v>3</v>
+        <v>-1024</v>
       </c>
     </row>
     <row r="1026" spans="1:14" x14ac:dyDescent="0.25">
@@ -35973,7 +35973,7 @@
         <v>FFD</v>
       </c>
       <c r="N1027" s="15">
-        <f t="shared" ref="N1027:N1090" si="120">IF((MOD(ROW(K1027)-2,3)=0), K1027, 9999)</f>
+        <f t="shared" ref="N1027:N1090" si="120">IF((MOD(ROW(I1027)-2,3)=0), I1027, 9999)</f>
         <v>9999</v>
       </c>
     </row>
@@ -36007,7 +36007,7 @@
       </c>
       <c r="N1028" s="15">
         <f t="shared" si="120"/>
-        <v>-6</v>
+        <v>-1024</v>
       </c>
     </row>
     <row r="1029" spans="1:14" x14ac:dyDescent="0.25">
@@ -36106,7 +36106,7 @@
       </c>
       <c r="N1031" s="15">
         <f t="shared" si="120"/>
-        <v>-16</v>
+        <v>-1024</v>
       </c>
     </row>
     <row r="1032" spans="1:14" x14ac:dyDescent="0.25">
@@ -36205,7 +36205,7 @@
       </c>
       <c r="N1034" s="15">
         <f t="shared" si="120"/>
-        <v>-25</v>
+        <v>-1024</v>
       </c>
     </row>
     <row r="1035" spans="1:14" x14ac:dyDescent="0.25">
@@ -36304,7 +36304,7 @@
       </c>
       <c r="N1037" s="15">
         <f t="shared" si="120"/>
-        <v>-35</v>
+        <v>-1023</v>
       </c>
     </row>
     <row r="1038" spans="1:14" x14ac:dyDescent="0.25">
@@ -36403,7 +36403,7 @@
       </c>
       <c r="N1040" s="15">
         <f t="shared" si="120"/>
-        <v>-44</v>
+        <v>-1023</v>
       </c>
     </row>
     <row r="1041" spans="1:14" x14ac:dyDescent="0.25">
@@ -36502,7 +36502,7 @@
       </c>
       <c r="N1043" s="15">
         <f t="shared" si="120"/>
-        <v>-53</v>
+        <v>-1023</v>
       </c>
     </row>
     <row r="1044" spans="1:14" x14ac:dyDescent="0.25">
@@ -36601,7 +36601,7 @@
       </c>
       <c r="N1046" s="15">
         <f t="shared" si="120"/>
-        <v>-63</v>
+        <v>-1022</v>
       </c>
     </row>
     <row r="1047" spans="1:14" x14ac:dyDescent="0.25">
@@ -36700,7 +36700,7 @@
       </c>
       <c r="N1049" s="15">
         <f t="shared" si="120"/>
-        <v>-72</v>
+        <v>-1021</v>
       </c>
     </row>
     <row r="1050" spans="1:14" x14ac:dyDescent="0.25">
@@ -36799,7 +36799,7 @@
       </c>
       <c r="N1052" s="15">
         <f t="shared" si="120"/>
-        <v>-82</v>
+        <v>-1021</v>
       </c>
     </row>
     <row r="1053" spans="1:14" x14ac:dyDescent="0.25">
@@ -36898,7 +36898,7 @@
       </c>
       <c r="N1055" s="15">
         <f t="shared" si="120"/>
-        <v>-91</v>
+        <v>-1020</v>
       </c>
     </row>
     <row r="1056" spans="1:14" x14ac:dyDescent="0.25">
@@ -36997,7 +36997,7 @@
       </c>
       <c r="N1058" s="15">
         <f t="shared" si="120"/>
-        <v>-100</v>
+        <v>-1019</v>
       </c>
     </row>
     <row r="1059" spans="1:14" x14ac:dyDescent="0.25">
@@ -37096,7 +37096,7 @@
       </c>
       <c r="N1061" s="15">
         <f t="shared" si="120"/>
-        <v>-110</v>
+        <v>-1018</v>
       </c>
     </row>
     <row r="1062" spans="1:14" x14ac:dyDescent="0.25">
@@ -37195,7 +37195,7 @@
       </c>
       <c r="N1064" s="15">
         <f t="shared" si="120"/>
-        <v>-119</v>
+        <v>-1017</v>
       </c>
     </row>
     <row r="1065" spans="1:14" x14ac:dyDescent="0.25">
@@ -37294,7 +37294,7 @@
       </c>
       <c r="N1067" s="15">
         <f t="shared" si="120"/>
-        <v>-128</v>
+        <v>-1016</v>
       </c>
     </row>
     <row r="1068" spans="1:14" x14ac:dyDescent="0.25">
@@ -37393,7 +37393,7 @@
       </c>
       <c r="N1070" s="15">
         <f t="shared" si="120"/>
-        <v>-138</v>
+        <v>-1015</v>
       </c>
     </row>
     <row r="1071" spans="1:14" x14ac:dyDescent="0.25">
@@ -37492,7 +37492,7 @@
       </c>
       <c r="N1073" s="15">
         <f t="shared" si="120"/>
-        <v>-147</v>
+        <v>-1013</v>
       </c>
     </row>
     <row r="1074" spans="1:14" x14ac:dyDescent="0.25">
@@ -37591,7 +37591,7 @@
       </c>
       <c r="N1076" s="15">
         <f t="shared" si="120"/>
-        <v>-156</v>
+        <v>-1012</v>
       </c>
     </row>
     <row r="1077" spans="1:14" x14ac:dyDescent="0.25">
@@ -37690,7 +37690,7 @@
       </c>
       <c r="N1079" s="15">
         <f t="shared" si="120"/>
-        <v>-166</v>
+        <v>-1010</v>
       </c>
     </row>
     <row r="1080" spans="1:14" x14ac:dyDescent="0.25">
@@ -37789,7 +37789,7 @@
       </c>
       <c r="N1082" s="15">
         <f t="shared" si="120"/>
-        <v>-175</v>
+        <v>-1009</v>
       </c>
     </row>
     <row r="1083" spans="1:14" x14ac:dyDescent="0.25">
@@ -37888,7 +37888,7 @@
       </c>
       <c r="N1085" s="15">
         <f t="shared" si="120"/>
-        <v>-184</v>
+        <v>-1007</v>
       </c>
     </row>
     <row r="1086" spans="1:14" x14ac:dyDescent="0.25">
@@ -37987,7 +37987,7 @@
       </c>
       <c r="N1088" s="15">
         <f t="shared" si="120"/>
-        <v>-194</v>
+        <v>-1006</v>
       </c>
     </row>
     <row r="1089" spans="1:14" x14ac:dyDescent="0.25">
@@ -38085,8 +38085,8 @@
         <v>F35</v>
       </c>
       <c r="N1091" s="15">
-        <f t="shared" ref="N1091:N1154" si="127">IF((MOD(ROW(K1091)-2,3)=0), K1091, 9999)</f>
-        <v>-203</v>
+        <f t="shared" ref="N1091:N1154" si="127">IF((MOD(ROW(I1091)-2,3)=0), I1091, 9999)</f>
+        <v>-1004</v>
       </c>
     </row>
     <row r="1092" spans="1:14" x14ac:dyDescent="0.25">
@@ -38185,7 +38185,7 @@
       </c>
       <c r="N1094" s="15">
         <f t="shared" si="127"/>
-        <v>-212</v>
+        <v>-1002</v>
       </c>
     </row>
     <row r="1095" spans="1:14" x14ac:dyDescent="0.25">
@@ -38284,7 +38284,7 @@
       </c>
       <c r="N1097" s="15">
         <f t="shared" si="127"/>
-        <v>-221</v>
+        <v>-1000</v>
       </c>
     </row>
     <row r="1098" spans="1:14" x14ac:dyDescent="0.25">
@@ -38383,7 +38383,7 @@
       </c>
       <c r="N1100" s="15">
         <f t="shared" si="127"/>
-        <v>-230</v>
+        <v>-998</v>
       </c>
     </row>
     <row r="1101" spans="1:14" x14ac:dyDescent="0.25">
@@ -38482,7 +38482,7 @@
       </c>
       <c r="N1103" s="15">
         <f t="shared" si="127"/>
-        <v>-240</v>
+        <v>-996</v>
       </c>
     </row>
     <row r="1104" spans="1:14" x14ac:dyDescent="0.25">
@@ -38581,7 +38581,7 @@
       </c>
       <c r="N1106" s="15">
         <f t="shared" si="127"/>
-        <v>-249</v>
+        <v>-993</v>
       </c>
     </row>
     <row r="1107" spans="1:14" x14ac:dyDescent="0.25">
@@ -38680,7 +38680,7 @@
       </c>
       <c r="N1109" s="15">
         <f t="shared" si="127"/>
-        <v>-258</v>
+        <v>-991</v>
       </c>
     </row>
     <row r="1110" spans="1:14" x14ac:dyDescent="0.25">
@@ -38779,7 +38779,7 @@
       </c>
       <c r="N1112" s="15">
         <f t="shared" si="127"/>
-        <v>-267</v>
+        <v>-989</v>
       </c>
     </row>
     <row r="1113" spans="1:14" x14ac:dyDescent="0.25">
@@ -38878,7 +38878,7 @@
       </c>
       <c r="N1115" s="15">
         <f t="shared" si="127"/>
-        <v>-276</v>
+        <v>-986</v>
       </c>
     </row>
     <row r="1116" spans="1:14" x14ac:dyDescent="0.25">
@@ -38977,7 +38977,7 @@
       </c>
       <c r="N1118" s="15">
         <f t="shared" si="127"/>
-        <v>-285</v>
+        <v>-983</v>
       </c>
     </row>
     <row r="1119" spans="1:14" x14ac:dyDescent="0.25">
@@ -39076,7 +39076,7 @@
       </c>
       <c r="N1121" s="15">
         <f t="shared" si="127"/>
-        <v>-294</v>
+        <v>-981</v>
       </c>
     </row>
     <row r="1122" spans="1:14" x14ac:dyDescent="0.25">
@@ -39175,7 +39175,7 @@
       </c>
       <c r="N1124" s="15">
         <f t="shared" si="127"/>
-        <v>-303</v>
+        <v>-978</v>
       </c>
     </row>
     <row r="1125" spans="1:14" x14ac:dyDescent="0.25">
@@ -39274,7 +39274,7 @@
       </c>
       <c r="N1127" s="15">
         <f t="shared" si="127"/>
-        <v>-312</v>
+        <v>-975</v>
       </c>
     </row>
     <row r="1128" spans="1:14" x14ac:dyDescent="0.25">
@@ -39373,7 +39373,7 @@
       </c>
       <c r="N1130" s="15">
         <f t="shared" si="127"/>
-        <v>-321</v>
+        <v>-972</v>
       </c>
     </row>
     <row r="1131" spans="1:14" x14ac:dyDescent="0.25">
@@ -39472,7 +39472,7 @@
       </c>
       <c r="N1133" s="15">
         <f t="shared" si="127"/>
-        <v>-330</v>
+        <v>-969</v>
       </c>
     </row>
     <row r="1134" spans="1:14" x14ac:dyDescent="0.25">
@@ -39571,7 +39571,7 @@
       </c>
       <c r="N1136" s="15">
         <f t="shared" si="127"/>
-        <v>-339</v>
+        <v>-966</v>
       </c>
     </row>
     <row r="1137" spans="1:14" x14ac:dyDescent="0.25">
@@ -39670,7 +39670,7 @@
       </c>
       <c r="N1139" s="15">
         <f t="shared" si="127"/>
-        <v>-348</v>
+        <v>-963</v>
       </c>
     </row>
     <row r="1140" spans="1:14" x14ac:dyDescent="0.25">
@@ -39769,7 +39769,7 @@
       </c>
       <c r="N1142" s="15">
         <f t="shared" si="127"/>
-        <v>-357</v>
+        <v>-960</v>
       </c>
     </row>
     <row r="1143" spans="1:14" x14ac:dyDescent="0.25">
@@ -39868,7 +39868,7 @@
       </c>
       <c r="N1145" s="15">
         <f t="shared" si="127"/>
-        <v>-366</v>
+        <v>-957</v>
       </c>
     </row>
     <row r="1146" spans="1:14" x14ac:dyDescent="0.25">
@@ -39967,7 +39967,7 @@
       </c>
       <c r="N1148" s="15">
         <f t="shared" si="127"/>
-        <v>-374</v>
+        <v>-953</v>
       </c>
     </row>
     <row r="1149" spans="1:14" x14ac:dyDescent="0.25">
@@ -40066,7 +40066,7 @@
       </c>
       <c r="N1151" s="15">
         <f t="shared" si="127"/>
-        <v>-383</v>
+        <v>-950</v>
       </c>
     </row>
     <row r="1152" spans="1:14" x14ac:dyDescent="0.25">
@@ -40165,7 +40165,7 @@
       </c>
       <c r="N1154" s="15">
         <f t="shared" si="127"/>
-        <v>-392</v>
+        <v>-946</v>
       </c>
     </row>
     <row r="1155" spans="1:14" x14ac:dyDescent="0.25">
@@ -40197,7 +40197,7 @@
         <v>E75</v>
       </c>
       <c r="N1155" s="15">
-        <f t="shared" ref="N1155:N1218" si="134">IF((MOD(ROW(K1155)-2,3)=0), K1155, 9999)</f>
+        <f t="shared" ref="N1155:N1218" si="134">IF((MOD(ROW(I1155)-2,3)=0), I1155, 9999)</f>
         <v>9999</v>
       </c>
     </row>
@@ -40264,7 +40264,7 @@
       </c>
       <c r="N1157" s="15">
         <f t="shared" si="134"/>
-        <v>-401</v>
+        <v>-942</v>
       </c>
     </row>
     <row r="1158" spans="1:14" x14ac:dyDescent="0.25">
@@ -40363,7 +40363,7 @@
       </c>
       <c r="N1160" s="15">
         <f t="shared" si="134"/>
-        <v>-409</v>
+        <v>-939</v>
       </c>
     </row>
     <row r="1161" spans="1:14" x14ac:dyDescent="0.25">
@@ -40462,7 +40462,7 @@
       </c>
       <c r="N1163" s="15">
         <f t="shared" si="134"/>
-        <v>-418</v>
+        <v>-935</v>
       </c>
     </row>
     <row r="1164" spans="1:14" x14ac:dyDescent="0.25">
@@ -40561,7 +40561,7 @@
       </c>
       <c r="N1166" s="15">
         <f t="shared" si="134"/>
-        <v>-426</v>
+        <v>-931</v>
       </c>
     </row>
     <row r="1167" spans="1:14" x14ac:dyDescent="0.25">
@@ -40660,7 +40660,7 @@
       </c>
       <c r="N1169" s="15">
         <f t="shared" si="134"/>
-        <v>-435</v>
+        <v>-927</v>
       </c>
     </row>
     <row r="1170" spans="1:14" x14ac:dyDescent="0.25">
@@ -40759,7 +40759,7 @@
       </c>
       <c r="N1172" s="15">
         <f t="shared" si="134"/>
-        <v>-443</v>
+        <v>-923</v>
       </c>
     </row>
     <row r="1173" spans="1:14" x14ac:dyDescent="0.25">
@@ -40858,7 +40858,7 @@
       </c>
       <c r="N1175" s="15">
         <f t="shared" si="134"/>
-        <v>-452</v>
+        <v>-919</v>
       </c>
     </row>
     <row r="1176" spans="1:14" x14ac:dyDescent="0.25">
@@ -40957,7 +40957,7 @@
       </c>
       <c r="N1178" s="15">
         <f t="shared" si="134"/>
-        <v>-460</v>
+        <v>-915</v>
       </c>
     </row>
     <row r="1179" spans="1:14" x14ac:dyDescent="0.25">
@@ -41056,7 +41056,7 @@
       </c>
       <c r="N1181" s="15">
         <f t="shared" si="134"/>
-        <v>-469</v>
+        <v>-910</v>
       </c>
     </row>
     <row r="1182" spans="1:14" x14ac:dyDescent="0.25">
@@ -41155,7 +41155,7 @@
       </c>
       <c r="N1184" s="15">
         <f t="shared" si="134"/>
-        <v>-477</v>
+        <v>-906</v>
       </c>
     </row>
     <row r="1185" spans="1:14" x14ac:dyDescent="0.25">
@@ -41254,7 +41254,7 @@
       </c>
       <c r="N1187" s="15">
         <f t="shared" si="134"/>
-        <v>-485</v>
+        <v>-902</v>
       </c>
     </row>
     <row r="1188" spans="1:14" x14ac:dyDescent="0.25">
@@ -41353,7 +41353,7 @@
       </c>
       <c r="N1190" s="15">
         <f t="shared" si="134"/>
-        <v>-494</v>
+        <v>-897</v>
       </c>
     </row>
     <row r="1191" spans="1:14" x14ac:dyDescent="0.25">
@@ -41452,7 +41452,7 @@
       </c>
       <c r="N1193" s="15">
         <f t="shared" si="134"/>
-        <v>-502</v>
+        <v>-893</v>
       </c>
     </row>
     <row r="1194" spans="1:14" x14ac:dyDescent="0.25">
@@ -41551,7 +41551,7 @@
       </c>
       <c r="N1196" s="15">
         <f t="shared" si="134"/>
-        <v>-510</v>
+        <v>-888</v>
       </c>
     </row>
     <row r="1197" spans="1:14" x14ac:dyDescent="0.25">
@@ -41650,7 +41650,7 @@
       </c>
       <c r="N1199" s="15">
         <f t="shared" si="134"/>
-        <v>-518</v>
+        <v>-883</v>
       </c>
     </row>
     <row r="1200" spans="1:14" x14ac:dyDescent="0.25">
@@ -41749,7 +41749,7 @@
       </c>
       <c r="N1202" s="15">
         <f t="shared" si="134"/>
-        <v>-526</v>
+        <v>-878</v>
       </c>
     </row>
     <row r="1203" spans="1:14" x14ac:dyDescent="0.25">
@@ -41848,7 +41848,7 @@
       </c>
       <c r="N1205" s="15">
         <f t="shared" si="134"/>
-        <v>-535</v>
+        <v>-873</v>
       </c>
     </row>
     <row r="1206" spans="1:14" x14ac:dyDescent="0.25">
@@ -41947,7 +41947,7 @@
       </c>
       <c r="N1208" s="15">
         <f t="shared" si="134"/>
-        <v>-543</v>
+        <v>-868</v>
       </c>
     </row>
     <row r="1209" spans="1:14" x14ac:dyDescent="0.25">
@@ -42046,7 +42046,7 @@
       </c>
       <c r="N1211" s="15">
         <f t="shared" si="134"/>
-        <v>-550</v>
+        <v>-863</v>
       </c>
     </row>
     <row r="1212" spans="1:14" x14ac:dyDescent="0.25">
@@ -42145,7 +42145,7 @@
       </c>
       <c r="N1214" s="15">
         <f t="shared" si="134"/>
-        <v>-558</v>
+        <v>-858</v>
       </c>
     </row>
     <row r="1215" spans="1:14" x14ac:dyDescent="0.25">
@@ -42244,7 +42244,7 @@
       </c>
       <c r="N1217" s="15">
         <f t="shared" si="134"/>
-        <v>-566</v>
+        <v>-853</v>
       </c>
     </row>
     <row r="1218" spans="1:14" x14ac:dyDescent="0.25">
@@ -42309,7 +42309,7 @@
         <v>DC4</v>
       </c>
       <c r="N1219" s="15">
-        <f t="shared" ref="N1219:N1282" si="141">IF((MOD(ROW(K1219)-2,3)=0), K1219, 9999)</f>
+        <f t="shared" ref="N1219:N1282" si="141">IF((MOD(ROW(I1219)-2,3)=0), I1219, 9999)</f>
         <v>9999</v>
       </c>
     </row>
@@ -42343,7 +42343,7 @@
       </c>
       <c r="N1220" s="15">
         <f t="shared" si="141"/>
-        <v>-574</v>
+        <v>-848</v>
       </c>
     </row>
     <row r="1221" spans="1:14" x14ac:dyDescent="0.25">
@@ -42442,7 +42442,7 @@
       </c>
       <c r="N1223" s="15">
         <f t="shared" si="141"/>
-        <v>-582</v>
+        <v>-843</v>
       </c>
     </row>
     <row r="1224" spans="1:14" x14ac:dyDescent="0.25">
@@ -42541,7 +42541,7 @@
       </c>
       <c r="N1226" s="15">
         <f t="shared" si="141"/>
-        <v>-590</v>
+        <v>-837</v>
       </c>
     </row>
     <row r="1227" spans="1:14" x14ac:dyDescent="0.25">
@@ -42640,7 +42640,7 @@
       </c>
       <c r="N1229" s="15">
         <f t="shared" si="141"/>
-        <v>-597</v>
+        <v>-832</v>
       </c>
     </row>
     <row r="1230" spans="1:14" x14ac:dyDescent="0.25">
@@ -42739,7 +42739,7 @@
       </c>
       <c r="N1232" s="15">
         <f t="shared" si="141"/>
-        <v>-605</v>
+        <v>-826</v>
       </c>
     </row>
     <row r="1233" spans="1:14" x14ac:dyDescent="0.25">
@@ -42838,7 +42838,7 @@
       </c>
       <c r="N1235" s="15">
         <f t="shared" si="141"/>
-        <v>-613</v>
+        <v>-821</v>
       </c>
     </row>
     <row r="1236" spans="1:14" x14ac:dyDescent="0.25">
@@ -42937,7 +42937,7 @@
       </c>
       <c r="N1238" s="15">
         <f t="shared" si="141"/>
-        <v>-620</v>
+        <v>-815</v>
       </c>
     </row>
     <row r="1239" spans="1:14" x14ac:dyDescent="0.25">
@@ -43036,7 +43036,7 @@
       </c>
       <c r="N1241" s="15">
         <f t="shared" si="141"/>
-        <v>-628</v>
+        <v>-809</v>
       </c>
     </row>
     <row r="1242" spans="1:14" x14ac:dyDescent="0.25">
@@ -43135,7 +43135,7 @@
       </c>
       <c r="N1244" s="15">
         <f t="shared" si="141"/>
-        <v>-635</v>
+        <v>-803</v>
       </c>
     </row>
     <row r="1245" spans="1:14" x14ac:dyDescent="0.25">
@@ -43234,7 +43234,7 @@
       </c>
       <c r="N1247" s="15">
         <f t="shared" si="141"/>
-        <v>-642</v>
+        <v>-798</v>
       </c>
     </row>
     <row r="1248" spans="1:14" x14ac:dyDescent="0.25">
@@ -43333,7 +43333,7 @@
       </c>
       <c r="N1250" s="15">
         <f t="shared" si="141"/>
-        <v>-650</v>
+        <v>-792</v>
       </c>
     </row>
     <row r="1251" spans="1:14" x14ac:dyDescent="0.25">
@@ -43432,7 +43432,7 @@
       </c>
       <c r="N1253" s="15">
         <f t="shared" si="141"/>
-        <v>-657</v>
+        <v>-786</v>
       </c>
     </row>
     <row r="1254" spans="1:14" x14ac:dyDescent="0.25">
@@ -43531,7 +43531,7 @@
       </c>
       <c r="N1256" s="15">
         <f t="shared" si="141"/>
-        <v>-664</v>
+        <v>-779</v>
       </c>
     </row>
     <row r="1257" spans="1:14" x14ac:dyDescent="0.25">
@@ -43630,7 +43630,7 @@
       </c>
       <c r="N1259" s="15">
         <f t="shared" si="141"/>
-        <v>-671</v>
+        <v>-773</v>
       </c>
     </row>
     <row r="1260" spans="1:14" x14ac:dyDescent="0.25">
@@ -43729,7 +43729,7 @@
       </c>
       <c r="N1262" s="15">
         <f t="shared" si="141"/>
-        <v>-678</v>
+        <v>-767</v>
       </c>
     </row>
     <row r="1263" spans="1:14" x14ac:dyDescent="0.25">
@@ -43828,7 +43828,7 @@
       </c>
       <c r="N1265" s="15">
         <f t="shared" si="141"/>
-        <v>-685</v>
+        <v>-761</v>
       </c>
     </row>
     <row r="1266" spans="1:14" x14ac:dyDescent="0.25">
@@ -43927,7 +43927,7 @@
       </c>
       <c r="N1268" s="15">
         <f t="shared" si="141"/>
-        <v>-692</v>
+        <v>-755</v>
       </c>
     </row>
     <row r="1269" spans="1:14" x14ac:dyDescent="0.25">
@@ -44026,7 +44026,7 @@
       </c>
       <c r="N1271" s="15">
         <f t="shared" si="141"/>
-        <v>-699</v>
+        <v>-748</v>
       </c>
     </row>
     <row r="1272" spans="1:14" x14ac:dyDescent="0.25">
@@ -44125,7 +44125,7 @@
       </c>
       <c r="N1274" s="15">
         <f t="shared" si="141"/>
-        <v>-706</v>
+        <v>-742</v>
       </c>
     </row>
     <row r="1275" spans="1:14" x14ac:dyDescent="0.25">
@@ -44224,7 +44224,7 @@
       </c>
       <c r="N1277" s="15">
         <f t="shared" si="141"/>
-        <v>-713</v>
+        <v>-735</v>
       </c>
     </row>
     <row r="1278" spans="1:14" x14ac:dyDescent="0.25">
@@ -44323,7 +44323,7 @@
       </c>
       <c r="N1280" s="15">
         <f t="shared" si="141"/>
-        <v>-720</v>
+        <v>-729</v>
       </c>
     </row>
     <row r="1281" spans="1:14" x14ac:dyDescent="0.25">
@@ -44421,8 +44421,8 @@
         <v>D2A</v>
       </c>
       <c r="N1283" s="15">
-        <f t="shared" ref="N1283:N1346" si="148">IF((MOD(ROW(K1283)-2,3)=0), K1283, 9999)</f>
-        <v>-726</v>
+        <f t="shared" ref="N1283:N1346" si="148">IF((MOD(ROW(I1283)-2,3)=0), I1283, 9999)</f>
+        <v>-722</v>
       </c>
     </row>
     <row r="1284" spans="1:14" x14ac:dyDescent="0.25">
@@ -44521,7 +44521,7 @@
       </c>
       <c r="N1286" s="15">
         <f t="shared" si="148"/>
-        <v>-733</v>
+        <v>-715</v>
       </c>
     </row>
     <row r="1287" spans="1:14" x14ac:dyDescent="0.25">
@@ -44620,7 +44620,7 @@
       </c>
       <c r="N1289" s="15">
         <f t="shared" si="148"/>
-        <v>-739</v>
+        <v>-708</v>
       </c>
     </row>
     <row r="1290" spans="1:14" x14ac:dyDescent="0.25">
@@ -44719,7 +44719,7 @@
       </c>
       <c r="N1292" s="15">
         <f t="shared" si="148"/>
-        <v>-746</v>
+        <v>-702</v>
       </c>
     </row>
     <row r="1293" spans="1:14" x14ac:dyDescent="0.25">
@@ -44818,7 +44818,7 @@
       </c>
       <c r="N1295" s="15">
         <f t="shared" si="148"/>
-        <v>-752</v>
+        <v>-695</v>
       </c>
     </row>
     <row r="1296" spans="1:14" x14ac:dyDescent="0.25">
@@ -44917,7 +44917,7 @@
       </c>
       <c r="N1298" s="15">
         <f t="shared" si="148"/>
-        <v>-759</v>
+        <v>-688</v>
       </c>
     </row>
     <row r="1299" spans="1:14" x14ac:dyDescent="0.25">
@@ -45016,7 +45016,7 @@
       </c>
       <c r="N1301" s="15">
         <f t="shared" si="148"/>
-        <v>-765</v>
+        <v>-681</v>
       </c>
     </row>
     <row r="1302" spans="1:14" x14ac:dyDescent="0.25">
@@ -45115,7 +45115,7 @@
       </c>
       <c r="N1304" s="15">
         <f t="shared" si="148"/>
-        <v>-771</v>
+        <v>-674</v>
       </c>
     </row>
     <row r="1305" spans="1:14" x14ac:dyDescent="0.25">
@@ -45214,7 +45214,7 @@
       </c>
       <c r="N1307" s="15">
         <f t="shared" si="148"/>
-        <v>-777</v>
+        <v>-666</v>
       </c>
     </row>
     <row r="1308" spans="1:14" x14ac:dyDescent="0.25">
@@ -45313,7 +45313,7 @@
       </c>
       <c r="N1310" s="15">
         <f t="shared" si="148"/>
-        <v>-784</v>
+        <v>-659</v>
       </c>
     </row>
     <row r="1311" spans="1:14" x14ac:dyDescent="0.25">
@@ -45412,7 +45412,7 @@
       </c>
       <c r="N1313" s="15">
         <f t="shared" si="148"/>
-        <v>-790</v>
+        <v>-652</v>
       </c>
     </row>
     <row r="1314" spans="1:14" x14ac:dyDescent="0.25">
@@ -45511,7 +45511,7 @@
       </c>
       <c r="N1316" s="15">
         <f t="shared" si="148"/>
-        <v>-796</v>
+        <v>-645</v>
       </c>
     </row>
     <row r="1317" spans="1:14" x14ac:dyDescent="0.25">
@@ -45610,7 +45610,7 @@
       </c>
       <c r="N1319" s="15">
         <f t="shared" si="148"/>
-        <v>-801</v>
+        <v>-637</v>
       </c>
     </row>
     <row r="1320" spans="1:14" x14ac:dyDescent="0.25">
@@ -45709,7 +45709,7 @@
       </c>
       <c r="N1322" s="15">
         <f t="shared" si="148"/>
-        <v>-807</v>
+        <v>-630</v>
       </c>
     </row>
     <row r="1323" spans="1:14" x14ac:dyDescent="0.25">
@@ -45808,7 +45808,7 @@
       </c>
       <c r="N1325" s="15">
         <f t="shared" si="148"/>
-        <v>-813</v>
+        <v>-623</v>
       </c>
     </row>
     <row r="1326" spans="1:14" x14ac:dyDescent="0.25">
@@ -45907,7 +45907,7 @@
       </c>
       <c r="N1328" s="15">
         <f t="shared" si="148"/>
-        <v>-819</v>
+        <v>-615</v>
       </c>
     </row>
     <row r="1329" spans="1:14" x14ac:dyDescent="0.25">
@@ -46006,7 +46006,7 @@
       </c>
       <c r="N1331" s="15">
         <f t="shared" si="148"/>
-        <v>-824</v>
+        <v>-607</v>
       </c>
     </row>
     <row r="1332" spans="1:14" x14ac:dyDescent="0.25">
@@ -46105,7 +46105,7 @@
       </c>
       <c r="N1334" s="15">
         <f t="shared" si="148"/>
-        <v>-830</v>
+        <v>-600</v>
       </c>
     </row>
     <row r="1335" spans="1:14" x14ac:dyDescent="0.25">
@@ -46204,7 +46204,7 @@
       </c>
       <c r="N1337" s="15">
         <f t="shared" si="148"/>
-        <v>-835</v>
+        <v>-592</v>
       </c>
     </row>
     <row r="1338" spans="1:14" x14ac:dyDescent="0.25">
@@ -46303,7 +46303,7 @@
       </c>
       <c r="N1340" s="15">
         <f t="shared" si="148"/>
-        <v>-841</v>
+        <v>-584</v>
       </c>
     </row>
     <row r="1341" spans="1:14" x14ac:dyDescent="0.25">
@@ -46402,7 +46402,7 @@
       </c>
       <c r="N1343" s="15">
         <f t="shared" si="148"/>
-        <v>-846</v>
+        <v>-577</v>
       </c>
     </row>
     <row r="1344" spans="1:14" x14ac:dyDescent="0.25">
@@ -46501,7 +46501,7 @@
       </c>
       <c r="N1346" s="15">
         <f t="shared" si="148"/>
-        <v>-851</v>
+        <v>-569</v>
       </c>
     </row>
     <row r="1347" spans="1:14" x14ac:dyDescent="0.25">
@@ -46533,7 +46533,7 @@
         <v>CAB</v>
       </c>
       <c r="N1347" s="15">
-        <f t="shared" ref="N1347:N1410" si="155">IF((MOD(ROW(K1347)-2,3)=0), K1347, 9999)</f>
+        <f t="shared" ref="N1347:N1410" si="155">IF((MOD(ROW(I1347)-2,3)=0), I1347, 9999)</f>
         <v>9999</v>
       </c>
     </row>
@@ -46600,7 +46600,7 @@
       </c>
       <c r="N1349" s="15">
         <f t="shared" si="155"/>
-        <v>-857</v>
+        <v>-561</v>
       </c>
     </row>
     <row r="1350" spans="1:14" x14ac:dyDescent="0.25">
@@ -46699,7 +46699,7 @@
       </c>
       <c r="N1352" s="15">
         <f t="shared" si="155"/>
-        <v>-862</v>
+        <v>-553</v>
       </c>
     </row>
     <row r="1353" spans="1:14" x14ac:dyDescent="0.25">
@@ -46798,7 +46798,7 @@
       </c>
       <c r="N1355" s="15">
         <f t="shared" si="155"/>
-        <v>-867</v>
+        <v>-545</v>
       </c>
     </row>
     <row r="1356" spans="1:14" x14ac:dyDescent="0.25">
@@ -46897,7 +46897,7 @@
       </c>
       <c r="N1358" s="15">
         <f t="shared" si="155"/>
-        <v>-872</v>
+        <v>-537</v>
       </c>
     </row>
     <row r="1359" spans="1:14" x14ac:dyDescent="0.25">
@@ -46996,7 +46996,7 @@
       </c>
       <c r="N1361" s="15">
         <f t="shared" si="155"/>
-        <v>-877</v>
+        <v>-529</v>
       </c>
     </row>
     <row r="1362" spans="1:14" x14ac:dyDescent="0.25">
@@ -47095,7 +47095,7 @@
       </c>
       <c r="N1364" s="15">
         <f t="shared" si="155"/>
-        <v>-882</v>
+        <v>-521</v>
       </c>
     </row>
     <row r="1365" spans="1:14" x14ac:dyDescent="0.25">
@@ -47194,7 +47194,7 @@
       </c>
       <c r="N1367" s="15">
         <f t="shared" si="155"/>
-        <v>-886</v>
+        <v>-513</v>
       </c>
     </row>
     <row r="1368" spans="1:14" x14ac:dyDescent="0.25">
@@ -47293,7 +47293,7 @@
       </c>
       <c r="N1370" s="15">
         <f t="shared" si="155"/>
-        <v>-891</v>
+        <v>-505</v>
       </c>
     </row>
     <row r="1371" spans="1:14" x14ac:dyDescent="0.25">
@@ -47392,7 +47392,7 @@
       </c>
       <c r="N1373" s="15">
         <f t="shared" si="155"/>
-        <v>-896</v>
+        <v>-497</v>
       </c>
     </row>
     <row r="1374" spans="1:14" x14ac:dyDescent="0.25">
@@ -47491,7 +47491,7 @@
       </c>
       <c r="N1376" s="15">
         <f t="shared" si="155"/>
-        <v>-900</v>
+        <v>-488</v>
       </c>
     </row>
     <row r="1377" spans="1:14" x14ac:dyDescent="0.25">
@@ -47590,7 +47590,7 @@
       </c>
       <c r="N1379" s="15">
         <f t="shared" si="155"/>
-        <v>-905</v>
+        <v>-480</v>
       </c>
     </row>
     <row r="1380" spans="1:14" x14ac:dyDescent="0.25">
@@ -47689,7 +47689,7 @@
       </c>
       <c r="N1382" s="15">
         <f t="shared" si="155"/>
-        <v>-909</v>
+        <v>-472</v>
       </c>
     </row>
     <row r="1383" spans="1:14" x14ac:dyDescent="0.25">
@@ -47788,7 +47788,7 @@
       </c>
       <c r="N1385" s="15">
         <f t="shared" si="155"/>
-        <v>-913</v>
+        <v>-463</v>
       </c>
     </row>
     <row r="1386" spans="1:14" x14ac:dyDescent="0.25">
@@ -47887,7 +47887,7 @@
       </c>
       <c r="N1388" s="15">
         <f t="shared" si="155"/>
-        <v>-917</v>
+        <v>-455</v>
       </c>
     </row>
     <row r="1389" spans="1:14" x14ac:dyDescent="0.25">
@@ -47986,7 +47986,7 @@
       </c>
       <c r="N1391" s="15">
         <f t="shared" si="155"/>
-        <v>-922</v>
+        <v>-446</v>
       </c>
     </row>
     <row r="1392" spans="1:14" x14ac:dyDescent="0.25">
@@ -48085,7 +48085,7 @@
       </c>
       <c r="N1394" s="15">
         <f t="shared" si="155"/>
-        <v>-926</v>
+        <v>-438</v>
       </c>
     </row>
     <row r="1395" spans="1:14" x14ac:dyDescent="0.25">
@@ -48184,7 +48184,7 @@
       </c>
       <c r="N1397" s="15">
         <f t="shared" si="155"/>
-        <v>-930</v>
+        <v>-429</v>
       </c>
     </row>
     <row r="1398" spans="1:14" x14ac:dyDescent="0.25">
@@ -48283,7 +48283,7 @@
       </c>
       <c r="N1400" s="15">
         <f t="shared" si="155"/>
-        <v>-934</v>
+        <v>-421</v>
       </c>
     </row>
     <row r="1401" spans="1:14" x14ac:dyDescent="0.25">
@@ -48382,7 +48382,7 @@
       </c>
       <c r="N1403" s="15">
         <f t="shared" si="155"/>
-        <v>-937</v>
+        <v>-412</v>
       </c>
     </row>
     <row r="1404" spans="1:14" x14ac:dyDescent="0.25">
@@ -48481,7 +48481,7 @@
       </c>
       <c r="N1406" s="15">
         <f t="shared" si="155"/>
-        <v>-941</v>
+        <v>-403</v>
       </c>
     </row>
     <row r="1407" spans="1:14" x14ac:dyDescent="0.25">
@@ -48580,7 +48580,7 @@
       </c>
       <c r="N1409" s="15">
         <f t="shared" si="155"/>
-        <v>-945</v>
+        <v>-395</v>
       </c>
     </row>
     <row r="1410" spans="1:14" x14ac:dyDescent="0.25">
@@ -48645,7 +48645,7 @@
         <v>C4D</v>
       </c>
       <c r="N1411" s="15">
-        <f t="shared" ref="N1411:N1474" si="162">IF((MOD(ROW(K1411)-2,3)=0), K1411, 9999)</f>
+        <f t="shared" ref="N1411:N1474" si="162">IF((MOD(ROW(I1411)-2,3)=0), I1411, 9999)</f>
         <v>9999</v>
       </c>
     </row>
@@ -48679,7 +48679,7 @@
       </c>
       <c r="N1412" s="15">
         <f t="shared" si="162"/>
-        <v>-948</v>
+        <v>-386</v>
       </c>
     </row>
     <row r="1413" spans="1:14" x14ac:dyDescent="0.25">
@@ -48778,7 +48778,7 @@
       </c>
       <c r="N1415" s="15">
         <f t="shared" si="162"/>
-        <v>-952</v>
+        <v>-377</v>
       </c>
     </row>
     <row r="1416" spans="1:14" x14ac:dyDescent="0.25">
@@ -48877,7 +48877,7 @@
       </c>
       <c r="N1418" s="15">
         <f t="shared" si="162"/>
-        <v>-955</v>
+        <v>-369</v>
       </c>
     </row>
     <row r="1419" spans="1:14" x14ac:dyDescent="0.25">
@@ -48976,7 +48976,7 @@
       </c>
       <c r="N1421" s="15">
         <f t="shared" si="162"/>
-        <v>-959</v>
+        <v>-360</v>
       </c>
     </row>
     <row r="1422" spans="1:14" x14ac:dyDescent="0.25">
@@ -49075,7 +49075,7 @@
       </c>
       <c r="N1424" s="15">
         <f t="shared" si="162"/>
-        <v>-962</v>
+        <v>-351</v>
       </c>
     </row>
     <row r="1425" spans="1:14" x14ac:dyDescent="0.25">
@@ -49174,7 +49174,7 @@
       </c>
       <c r="N1427" s="15">
         <f t="shared" si="162"/>
-        <v>-965</v>
+        <v>-342</v>
       </c>
     </row>
     <row r="1428" spans="1:14" x14ac:dyDescent="0.25">
@@ -49273,7 +49273,7 @@
       </c>
       <c r="N1430" s="15">
         <f t="shared" si="162"/>
-        <v>-968</v>
+        <v>-333</v>
       </c>
     </row>
     <row r="1431" spans="1:14" x14ac:dyDescent="0.25">
@@ -49372,7 +49372,7 @@
       </c>
       <c r="N1433" s="15">
         <f t="shared" si="162"/>
-        <v>-971</v>
+        <v>-324</v>
       </c>
     </row>
     <row r="1434" spans="1:14" x14ac:dyDescent="0.25">
@@ -49471,7 +49471,7 @@
       </c>
       <c r="N1436" s="15">
         <f t="shared" si="162"/>
-        <v>-974</v>
+        <v>-315</v>
       </c>
     </row>
     <row r="1437" spans="1:14" x14ac:dyDescent="0.25">
@@ -49570,7 +49570,7 @@
       </c>
       <c r="N1439" s="15">
         <f t="shared" si="162"/>
-        <v>-977</v>
+        <v>-306</v>
       </c>
     </row>
     <row r="1440" spans="1:14" x14ac:dyDescent="0.25">
@@ -49669,7 +49669,7 @@
       </c>
       <c r="N1442" s="15">
         <f t="shared" si="162"/>
-        <v>-980</v>
+        <v>-297</v>
       </c>
     </row>
     <row r="1443" spans="1:14" x14ac:dyDescent="0.25">
@@ -49768,7 +49768,7 @@
       </c>
       <c r="N1445" s="15">
         <f t="shared" si="162"/>
-        <v>-983</v>
+        <v>-288</v>
       </c>
     </row>
     <row r="1446" spans="1:14" x14ac:dyDescent="0.25">
@@ -49867,7 +49867,7 @@
       </c>
       <c r="N1448" s="15">
         <f t="shared" si="162"/>
-        <v>-985</v>
+        <v>-279</v>
       </c>
     </row>
     <row r="1449" spans="1:14" x14ac:dyDescent="0.25">
@@ -49966,7 +49966,7 @@
       </c>
       <c r="N1451" s="15">
         <f t="shared" si="162"/>
-        <v>-988</v>
+        <v>-270</v>
       </c>
     </row>
     <row r="1452" spans="1:14" x14ac:dyDescent="0.25">
@@ -50065,7 +50065,7 @@
       </c>
       <c r="N1454" s="15">
         <f t="shared" si="162"/>
-        <v>-990</v>
+        <v>-261</v>
       </c>
     </row>
     <row r="1455" spans="1:14" x14ac:dyDescent="0.25">
@@ -50164,7 +50164,7 @@
       </c>
       <c r="N1457" s="15">
         <f t="shared" si="162"/>
-        <v>-993</v>
+        <v>-252</v>
       </c>
     </row>
     <row r="1458" spans="1:14" x14ac:dyDescent="0.25">
@@ -50263,7 +50263,7 @@
       </c>
       <c r="N1460" s="15">
         <f t="shared" si="162"/>
-        <v>-995</v>
+        <v>-243</v>
       </c>
     </row>
     <row r="1461" spans="1:14" x14ac:dyDescent="0.25">
@@ -50362,7 +50362,7 @@
       </c>
       <c r="N1463" s="15">
         <f t="shared" si="162"/>
-        <v>-997</v>
+        <v>-234</v>
       </c>
     </row>
     <row r="1464" spans="1:14" x14ac:dyDescent="0.25">
@@ -50461,7 +50461,7 @@
       </c>
       <c r="N1466" s="15">
         <f t="shared" si="162"/>
-        <v>-999</v>
+        <v>-224</v>
       </c>
     </row>
     <row r="1467" spans="1:14" x14ac:dyDescent="0.25">
@@ -50560,7 +50560,7 @@
       </c>
       <c r="N1469" s="15">
         <f t="shared" si="162"/>
-        <v>-1001</v>
+        <v>-215</v>
       </c>
     </row>
     <row r="1470" spans="1:14" x14ac:dyDescent="0.25">
@@ -50659,7 +50659,7 @@
       </c>
       <c r="N1472" s="15">
         <f t="shared" si="162"/>
-        <v>-1003</v>
+        <v>-206</v>
       </c>
     </row>
     <row r="1473" spans="1:14" x14ac:dyDescent="0.25">
@@ -50757,8 +50757,8 @@
         <v>C13</v>
       </c>
       <c r="N1475" s="15">
-        <f t="shared" ref="N1475:N1536" si="169">IF((MOD(ROW(K1475)-2,3)=0), K1475, 9999)</f>
-        <v>-1005</v>
+        <f t="shared" ref="N1475:N1537" si="169">IF((MOD(ROW(I1475)-2,3)=0), I1475, 9999)</f>
+        <v>-197</v>
       </c>
     </row>
     <row r="1476" spans="1:14" x14ac:dyDescent="0.25">
@@ -50857,7 +50857,7 @@
       </c>
       <c r="N1478" s="15">
         <f t="shared" si="169"/>
-        <v>-1007</v>
+        <v>-187</v>
       </c>
     </row>
     <row r="1479" spans="1:14" x14ac:dyDescent="0.25">
@@ -50956,7 +50956,7 @@
       </c>
       <c r="N1481" s="15">
         <f t="shared" si="169"/>
-        <v>-1008</v>
+        <v>-178</v>
       </c>
     </row>
     <row r="1482" spans="1:14" x14ac:dyDescent="0.25">
@@ -51055,7 +51055,7 @@
       </c>
       <c r="N1484" s="15">
         <f t="shared" si="169"/>
-        <v>-1010</v>
+        <v>-169</v>
       </c>
     </row>
     <row r="1485" spans="1:14" x14ac:dyDescent="0.25">
@@ -51154,7 +51154,7 @@
       </c>
       <c r="N1487" s="15">
         <f t="shared" si="169"/>
-        <v>-1011</v>
+        <v>-160</v>
       </c>
     </row>
     <row r="1488" spans="1:14" x14ac:dyDescent="0.25">
@@ -51253,7 +51253,7 @@
       </c>
       <c r="N1490" s="15">
         <f t="shared" si="169"/>
-        <v>-1013</v>
+        <v>-150</v>
       </c>
     </row>
     <row r="1491" spans="1:14" x14ac:dyDescent="0.25">
@@ -51352,7 +51352,7 @@
       </c>
       <c r="N1493" s="15">
         <f t="shared" si="169"/>
-        <v>-1014</v>
+        <v>-141</v>
       </c>
     </row>
     <row r="1494" spans="1:14" x14ac:dyDescent="0.25">
@@ -51451,7 +51451,7 @@
       </c>
       <c r="N1496" s="15">
         <f t="shared" si="169"/>
-        <v>-1016</v>
+        <v>-132</v>
       </c>
     </row>
     <row r="1497" spans="1:14" x14ac:dyDescent="0.25">
@@ -51550,7 +51550,7 @@
       </c>
       <c r="N1499" s="15">
         <f t="shared" si="169"/>
-        <v>-1017</v>
+        <v>-122</v>
       </c>
     </row>
     <row r="1500" spans="1:14" x14ac:dyDescent="0.25">
@@ -51649,7 +51649,7 @@
       </c>
       <c r="N1502" s="15">
         <f t="shared" si="169"/>
-        <v>-1018</v>
+        <v>-113</v>
       </c>
     </row>
     <row r="1503" spans="1:14" x14ac:dyDescent="0.25">
@@ -51748,7 +51748,7 @@
       </c>
       <c r="N1505" s="15">
         <f t="shared" si="169"/>
-        <v>-1019</v>
+        <v>-103</v>
       </c>
     </row>
     <row r="1506" spans="1:14" x14ac:dyDescent="0.25">
@@ -51847,7 +51847,7 @@
       </c>
       <c r="N1508" s="15">
         <f t="shared" si="169"/>
-        <v>-1020</v>
+        <v>-94</v>
       </c>
     </row>
     <row r="1509" spans="1:14" x14ac:dyDescent="0.25">
@@ -51946,7 +51946,7 @@
       </c>
       <c r="N1511" s="15">
         <f t="shared" si="169"/>
-        <v>-1020</v>
+        <v>-85</v>
       </c>
     </row>
     <row r="1512" spans="1:14" x14ac:dyDescent="0.25">
@@ -52045,7 +52045,7 @@
       </c>
       <c r="N1514" s="15">
         <f t="shared" si="169"/>
-        <v>-1021</v>
+        <v>-75</v>
       </c>
     </row>
     <row r="1515" spans="1:14" x14ac:dyDescent="0.25">
@@ -52144,7 +52144,7 @@
       </c>
       <c r="N1517" s="15">
         <f t="shared" si="169"/>
-        <v>-1022</v>
+        <v>-66</v>
       </c>
     </row>
     <row r="1518" spans="1:14" x14ac:dyDescent="0.25">
@@ -52243,7 +52243,7 @@
       </c>
       <c r="N1520" s="15">
         <f t="shared" si="169"/>
-        <v>-1022</v>
+        <v>-57</v>
       </c>
     </row>
     <row r="1521" spans="1:14" x14ac:dyDescent="0.25">
@@ -52342,7 +52342,7 @@
       </c>
       <c r="N1523" s="15">
         <f t="shared" si="169"/>
-        <v>-1023</v>
+        <v>-47</v>
       </c>
     </row>
     <row r="1524" spans="1:14" x14ac:dyDescent="0.25">
@@ -52441,7 +52441,7 @@
       </c>
       <c r="N1526" s="15">
         <f t="shared" si="169"/>
-        <v>-1023</v>
+        <v>-38</v>
       </c>
     </row>
     <row r="1527" spans="1:14" x14ac:dyDescent="0.25">
@@ -52540,7 +52540,7 @@
       </c>
       <c r="N1529" s="15">
         <f t="shared" si="169"/>
-        <v>-1024</v>
+        <v>-28</v>
       </c>
     </row>
     <row r="1530" spans="1:14" x14ac:dyDescent="0.25">
@@ -52639,7 +52639,7 @@
       </c>
       <c r="N1532" s="15">
         <f t="shared" si="169"/>
-        <v>-1024</v>
+        <v>-19</v>
       </c>
     </row>
     <row r="1533" spans="1:14" x14ac:dyDescent="0.25">
@@ -52738,7 +52738,7 @@
       </c>
       <c r="N1535" s="15">
         <f t="shared" si="169"/>
-        <v>-1024</v>
+        <v>-9</v>
       </c>
     </row>
     <row r="1536" spans="1:14" x14ac:dyDescent="0.25">
@@ -52803,7 +52803,7 @@
         <v>C00</v>
       </c>
       <c r="N1537" s="15">
-        <f>IF((MOD(ROW(K1537)-2,3)=0), K1537, 9999)</f>
+        <f t="shared" si="169"/>
         <v>9999</v>
       </c>
     </row>

</xml_diff>